<commit_message>
update report with US02/US03
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="181">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>eswaminathan</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -866,11 +869,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117705624"/>
-        <c:axId val="2117708696"/>
+        <c:axId val="2124482632"/>
+        <c:axId val="2124479448"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2117705624"/>
+        <c:axId val="2124482632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,14 +883,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117708696"/>
+        <c:crossAx val="2124479448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2117708696"/>
+        <c:axId val="2124479448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117705624"/>
+        <c:crossAx val="2124482632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,7 +1275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1741,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1870,6 +1873,15 @@
       <c r="F6">
         <v>20</v>
       </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
@@ -1886,6 +1898,15 @@
       </c>
       <c r="F7">
         <v>20</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:9">

</xml_diff>

<commit_message>
adding report and some additional changes for submission
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" r:id="rId4"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId5"/>
-    <sheet name="Burndown" sheetId="3" r:id="rId6"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId7"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId8"/>
-    <sheet name="Sprint3" sheetId="6" r:id="rId9"/>
-    <sheet name="Sprint4" sheetId="7" r:id="rId10"/>
-    <sheet name="Stories" sheetId="8" r:id="rId11"/>
+    <sheet name="Team" sheetId="1" r:id="rId1"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
+    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
+    <sheet name="Stories" sheetId="8" r:id="rId8"/>
   </sheets>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="172">
   <si>
     <t>Initials</t>
   </si>
@@ -86,7 +93,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="11"/>
         <rFont val="Verdana"/>
@@ -253,7 +260,6 @@
   <si>
     <t>Reject illegitimate dates</t>
   </si>
-  <si/>
   <si>
     <t>Date</t>
   </si>
@@ -535,59 +541,59 @@
   </si>
   <si>
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="m/d"/>
-    <numFmt numFmtId="60" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="3">
@@ -628,97 +634,144 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+  <cellStyleXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ff878787"/>
-      <rgbColor rgb="ff4a7dbb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF878787"/>
+      <rgbColor rgb="FF4A7DBB"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -727,7 +780,9 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="18"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -752,9 +807,6 @@
             <c:v>Series1</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
             <a:ln w="28575" cap="flat">
               <a:solidFill>
                 <a:srgbClr val="4A7EBB"/>
@@ -781,79 +833,59 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>'Burndown'!$A$2:$A$7</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Burndown!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2/9</c:v>
+                  <c:v>40947.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/23</c:v>
+                  <c:v>40961.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
+                <c:pt idx="2" formatCode="d\-mmm">
+                  <c:v>40968.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown'!$B$2:$B$7</c:f>
+              <c:f>Burndown!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:ptCount val="2"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.000000</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.000000</c:v>
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="2094734552"/>
-        <c:axId val="2094734553"/>
+        <c:smooth val="0"/>
+        <c:axId val="2075919720"/>
+        <c:axId val="2076676504"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="2094734552"/>
+      <c:dateAx>
+        <c:axId val="2075919720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -877,23 +909,24 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734553"/>
+        <c:crossAx val="2076676504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="2094734553"/>
+        <c:axId val="2076676504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,20 +961,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734552"/>
+        <c:crossAx val="2075919720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="6"/>
-        <c:minorUnit val="3"/>
+        <c:majorUnit val="6.0"/>
+        <c:minorUnit val="3.0"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -956,6 +990,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -970,11 +1005,16 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -988,18 +1028,18 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>126732</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1323779" y="1715050"/>
-        <a:ext cx="3842464" cy="2355033"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1009,7 +1049,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1135,7 +1175,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1144,7 +1184,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1153,7 +1193,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1227,7 +1267,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1235,7 +1275,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1254,7 +1294,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1284,7 +1324,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1310,7 +1350,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1336,7 +1376,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1362,7 +1402,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1388,7 +1428,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1414,7 +1454,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1440,7 +1480,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1466,7 +1506,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1492,7 +1532,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1505,9 +1545,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1522,7 +1568,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -1530,7 +1576,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1549,7 +1595,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1575,7 +1621,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1601,7 +1647,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1627,7 +1673,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1653,7 +1699,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1679,7 +1725,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1705,7 +1751,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1731,7 +1777,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1757,7 +1803,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1783,7 +1829,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1796,9 +1842,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1812,7 +1864,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1831,7 +1883,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1861,7 +1913,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1887,7 +1939,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1913,7 +1965,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1939,7 +1991,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1965,7 +2017,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1991,7 +2043,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2017,7 +2069,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2043,7 +2095,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2069,7 +2121,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2082,140 +2134,147 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.35156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="1" customWidth="1"/>
     <col min="6" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s" s="4">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="4">
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s" s="4">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s" s="4">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s" s="4">
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2224,329 +2283,360 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.35156" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.67188" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="5" customWidth="1"/>
-    <col min="4" max="4" width="6.67188" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.67188" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="5" customWidth="1"/>
     <col min="6" max="256" width="11" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
+      <c r="A2" s="3">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="3"/>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="6">
         <v>1</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s" s="4">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" t="s" s="4">
+      <c r="B9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" t="s" s="4">
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="C10" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" t="s" s="4">
+      <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s" s="4">
+      <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="6">
         <v>1</v>
       </c>
-      <c r="B12" t="s" s="4">
+      <c r="B12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s" s="4">
+      <c r="C12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s" s="4">
+      <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" t="s" s="4">
+      <c r="B13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s" s="4">
+      <c r="C13" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" t="s" s="4">
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s" s="4">
+      <c r="C14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" t="s" s="4">
+    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s" s="4">
+      <c r="C15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" t="s" s="4">
+      <c r="B16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s" s="4">
+      <c r="C16" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1">
       <c r="A17" s="6">
         <v>1</v>
       </c>
-      <c r="B17" t="s" s="4">
+      <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s" s="4">
+      <c r="C17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D17" t="s" s="4">
+      <c r="D17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1">
       <c r="A18" s="6">
         <v>1</v>
       </c>
-      <c r="B18" t="s" s="4">
+      <c r="B18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s" s="4">
+      <c r="C18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D18" t="s" s="4">
+      <c r="D18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" t="s" s="4">
+    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="A19" s="3">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C19" t="s" s="4">
+      <c r="C19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" t="s" s="4">
+    <row r="20" spans="1:5" ht="15" customHeight="1">
+      <c r="A20" s="3">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s" s="4">
+      <c r="C20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" t="s" s="4">
+    <row r="21" spans="1:5" ht="15" customHeight="1">
+      <c r="A21" s="3">
+        <v>2</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s" s="4">
+      <c r="C21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="3"/>
-      <c r="B22" t="s" s="4">
+      <c r="B22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s" s="4">
+      <c r="C22" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="3"/>
-      <c r="B23" t="s" s="4">
+      <c r="B23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s" s="4">
+      <c r="C23" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="3"/>
-      <c r="B24" t="s" s="4">
+      <c r="B24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s" s="4">
+      <c r="C24" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="3"/>
-      <c r="B25" t="s" s="4">
+      <c r="B25" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s" s="4">
+      <c r="C25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="3"/>
@@ -2554,53 +2644,59 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.6719" style="7" customWidth="1"/>
-    <col min="2" max="2" width="16.6719" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="7.17188" style="7" customWidth="1"/>
-    <col min="5" max="5" width="6.85156" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11" style="7" customWidth="1"/>
-    <col min="8" max="256" width="11" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
+    <col min="7" max="256" width="11" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s" s="2">
-        <v>81</v>
-      </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" ht="13.5" customHeight="1">
+    <row r="2" spans="1:7" ht="13.5" customHeight="1">
       <c r="A2" s="8">
         <v>40947</v>
       </c>
@@ -2615,7 +2711,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" ht="13.5" customHeight="1">
+    <row r="3" spans="1:7" ht="13.5" customHeight="1">
       <c r="A3" s="8">
         <v>40961</v>
       </c>
@@ -2634,20 +2730,28 @@
       </c>
       <c r="F3" s="10">
         <f>(D3-D2)/E3*60</f>
-        <v>125</v>
+        <v>125.00000000000001</v>
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    <row r="4" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A4" s="21">
+        <v>40968</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>269</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" ht="13.5" customHeight="1">
+    <row r="5" spans="1:7" ht="13.5" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2656,7 +2760,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" ht="13.5" customHeight="1">
+    <row r="6" spans="1:7" ht="13.5" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2665,7 +2769,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" ht="13.5" customHeight="1">
+    <row r="7" spans="1:7" ht="13.5" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2674,7 +2778,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" ht="13.5" customHeight="1">
+    <row r="8" spans="1:7" ht="13.5" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2683,7 +2787,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" ht="13.5" customHeight="1">
+    <row r="9" spans="1:7" ht="13.5" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2692,7 +2796,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" ht="13.5" customHeight="1">
+    <row r="10" spans="1:7" ht="13.5" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2701,7 +2805,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" ht="13.5" customHeight="1">
+    <row r="11" spans="1:7" ht="13.5" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2710,7 +2814,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" ht="13.5" customHeight="1">
+    <row r="12" spans="1:7" ht="13.5" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2719,7 +2823,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" ht="13.5" customHeight="1">
+    <row r="13" spans="1:7" ht="13.5" customHeight="1">
       <c r="A13" s="9"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2728,7 +2832,7 @@
       <c r="F13" s="9"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" ht="13.5" customHeight="1">
+    <row r="14" spans="1:7" ht="13.5" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2737,7 +2841,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" ht="13.5" customHeight="1">
+    <row r="15" spans="1:7" ht="13.5" customHeight="1">
       <c r="A15" s="9"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2746,7 +2850,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" ht="13.5" customHeight="1">
+    <row r="16" spans="1:7" ht="13.5" customHeight="1">
       <c r="A16" s="9"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2755,7 +2859,7 @@
       <c r="F16" s="9"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" ht="13.5" customHeight="1">
+    <row r="17" spans="1:7" ht="13.5" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2764,7 +2868,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" ht="13.5" customHeight="1">
+    <row r="18" spans="1:7" ht="13.5" customHeight="1">
       <c r="A18" s="9"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2773,7 +2877,7 @@
       <c r="F18" s="9"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" ht="13.5" customHeight="1">
+    <row r="19" spans="1:7" ht="13.5" customHeight="1">
       <c r="A19" s="9"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2782,7 +2886,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" ht="13.5" customHeight="1">
+    <row r="20" spans="1:7" ht="13.5" customHeight="1">
       <c r="A20" s="9"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2791,7 +2895,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" ht="13.5" customHeight="1">
+    <row r="21" spans="1:7" ht="13.5" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2800,7 +2904,7 @@
       <c r="F21" s="9"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" ht="13.5" customHeight="1">
+    <row r="22" spans="1:7" ht="13.5" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2809,7 +2913,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" ht="13.5" customHeight="1">
+    <row r="23" spans="1:7" ht="13.5" customHeight="1">
       <c r="A23" s="9"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2818,7 +2922,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" ht="13.5" customHeight="1">
+    <row r="24" spans="1:7" ht="13.5" customHeight="1">
       <c r="A24" s="9"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2827,7 +2931,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" ht="13.5" customHeight="1">
+    <row r="25" spans="1:7" ht="13.5" customHeight="1">
       <c r="A25" s="9"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2836,7 +2940,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" ht="13.5" customHeight="1">
+    <row r="26" spans="1:7" ht="13.5" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2847,74 +2951,82 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.67188" style="11" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="6.67188" style="11" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
     <col min="4" max="4" width="11" style="11" customWidth="1"/>
-    <col min="5" max="5" width="10.2891" style="11" customWidth="1"/>
-    <col min="6" max="6" width="10.3516" style="11" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.35156" style="11" customWidth="1"/>
-    <col min="9" max="9" width="10.6719" style="11" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="11" customWidth="1"/>
     <col min="10" max="256" width="11" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="12">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s" s="13">
+      <c r="E1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s" s="13">
+      <c r="G1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s" s="13">
+      <c r="H1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s" s="13">
+      <c r="I1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s" s="13">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E2" s="6">
         <v>7</v>
       </c>
@@ -2927,21 +3039,23 @@
       <c r="H2" s="6">
         <v>30</v>
       </c>
-      <c r="I2" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="I2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E3" s="6">
         <v>3</v>
       </c>
@@ -2954,21 +3068,23 @@
       <c r="H3" s="14">
         <v>10</v>
       </c>
-      <c r="I3" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="I3" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E4" s="6">
         <v>5</v>
       </c>
@@ -2981,21 +3097,23 @@
       <c r="H4" s="6">
         <v>60</v>
       </c>
-      <c r="I4" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="I4" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E5" s="6">
         <v>10</v>
       </c>
@@ -3008,21 +3126,23 @@
       <c r="H5" s="14">
         <v>40</v>
       </c>
-      <c r="I5" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
+      <c r="I5" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E6" s="6">
         <v>5</v>
       </c>
@@ -3035,21 +3155,23 @@
       <c r="H6" s="6">
         <v>60</v>
       </c>
-      <c r="I6" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
+      <c r="I6" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E7" s="6">
         <v>5</v>
       </c>
@@ -3062,11 +3184,11 @@
       <c r="H7" s="6">
         <v>5</v>
       </c>
-      <c r="I7" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
+      <c r="I7" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="15"/>
       <c r="C8" s="3"/>
@@ -3077,7 +3199,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="15"/>
       <c r="C9" s="3"/>
@@ -3088,7 +3210,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="15"/>
       <c r="C10" s="3"/>
@@ -3099,7 +3221,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="15"/>
       <c r="C11" s="3"/>
@@ -3110,7 +3232,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="15"/>
       <c r="C12" s="3"/>
@@ -3121,10 +3243,10 @@
       <c r="H12" s="3"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" t="s" s="12">
-        <v>88</v>
+      <c r="B13" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3134,7 +3256,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="12"/>
       <c r="C14" s="3"/>
@@ -3145,10 +3267,10 @@
       <c r="H14" s="3"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="3"/>
-      <c r="B15" t="s" s="12">
-        <v>89</v>
+      <c r="B15" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -3158,7 +3280,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="15"/>
       <c r="C16" s="3"/>
@@ -3169,7 +3291,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="15"/>
       <c r="C17" s="3"/>
@@ -3180,7 +3302,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="15"/>
       <c r="C18" s="3"/>
@@ -3191,10 +3313,10 @@
       <c r="H18" s="3"/>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="3"/>
-      <c r="B19" t="s" s="12">
-        <v>90</v>
+      <c r="B19" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -3206,63 +3328,288 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" style="16" customWidth="1"/>
-    <col min="2" max="2" width="11" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11" style="16" customWidth="1"/>
-    <col min="4" max="4" width="11" style="16" customWidth="1"/>
-    <col min="5" max="5" width="11" style="16" customWidth="1"/>
-    <col min="6" max="6" width="11" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11" style="16" customWidth="1"/>
-    <col min="8" max="8" width="11" style="16" customWidth="1"/>
-    <col min="9" max="9" width="11" style="16" customWidth="1"/>
-    <col min="10" max="256" width="11" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="256" width="11" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="27" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="12">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s" s="13">
+      <c r="E1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s" s="13">
+      <c r="G1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s" s="13">
+      <c r="H1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s" s="13">
+      <c r="I1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s" s="13">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="3">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="3">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3">
+        <v>60</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="3">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>60</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="3">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="256" width="11" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="27" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3273,7 +3620,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3284,7 +3631,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3295,7 +3642,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3306,7 +3653,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3317,7 +3664,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3328,7 +3675,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3339,7 +3686,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3350,7 +3697,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3363,63 +3710,59 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="17" customWidth="1"/>
-    <col min="2" max="2" width="11" style="17" customWidth="1"/>
-    <col min="3" max="3" width="11" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11" style="17" customWidth="1"/>
-    <col min="5" max="5" width="11" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11" style="17" customWidth="1"/>
-    <col min="8" max="8" width="11" style="17" customWidth="1"/>
-    <col min="9" max="9" width="11" style="17" customWidth="1"/>
-    <col min="10" max="256" width="11" style="17" customWidth="1"/>
+    <col min="1" max="256" width="11" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="27" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="12">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s" s="13">
+      <c r="E1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s" s="13">
+      <c r="G1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s" s="13">
+      <c r="H1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s" s="13">
+      <c r="I1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s" s="13">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3430,7 +3773,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3441,7 +3784,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3452,7 +3795,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3463,7 +3806,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3474,7 +3817,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3485,7 +3828,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3496,7 +3839,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3507,7 +3850,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3520,750 +3863,615 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="11" style="18" customWidth="1"/>
-    <col min="2" max="2" width="11" style="18" customWidth="1"/>
-    <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="4" width="11" style="18" customWidth="1"/>
-    <col min="5" max="5" width="11" style="18" customWidth="1"/>
-    <col min="6" max="6" width="11" style="18" customWidth="1"/>
-    <col min="7" max="7" width="11" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11" style="18" customWidth="1"/>
-    <col min="9" max="9" width="11" style="18" customWidth="1"/>
-    <col min="10" max="256" width="11" style="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="27" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s" s="12">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s" s="13">
-        <v>82</v>
-      </c>
-      <c r="F1" t="s" s="13">
-        <v>83</v>
-      </c>
-      <c r="G1" t="s" s="13">
-        <v>84</v>
-      </c>
-      <c r="H1" t="s" s="13">
-        <v>85</v>
-      </c>
-      <c r="I1" t="s" s="13">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV43"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" style="19" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="19" customWidth="1"/>
-    <col min="3" max="3" width="49.3516" style="19" customWidth="1"/>
-    <col min="4" max="4" width="11" style="19" customWidth="1"/>
-    <col min="5" max="5" width="11" style="19" customWidth="1"/>
-    <col min="6" max="256" width="11" style="19" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" style="19" customWidth="1"/>
+    <col min="4" max="256" width="11" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="12">
-        <v>91</v>
+      <c r="C1" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" ht="30" customHeight="1">
-      <c r="A2" t="s" s="4">
+    <row r="2" spans="1:5" ht="30" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s" s="20">
-        <v>92</v>
+      <c r="C2" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s" s="20">
+      <c r="C3" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s" s="4">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s" s="20">
+      <c r="D4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="30" customHeight="1">
-      <c r="A5" t="s" s="4">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s" s="4">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s" s="20">
-        <v>95</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s" s="20">
-        <v>96</v>
+      <c r="C6" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s" s="20">
-        <v>97</v>
+      <c r="C7" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" ht="45" customHeight="1">
-      <c r="A8" t="s" s="4">
+    <row r="8" spans="1:5" ht="45" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s" s="20">
+      <c r="C8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>98</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="30" customHeight="1">
-      <c r="A9" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s" s="20">
-        <v>99</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="30" customHeight="1">
-      <c r="A10" t="s" s="4">
+    <row r="10" spans="1:5" ht="30" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C10" t="s" s="20">
-        <v>100</v>
+      <c r="C10" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" ht="30" customHeight="1">
-      <c r="A11" t="s" s="4">
+    <row r="11" spans="1:5" ht="30" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s" s="4">
+      <c r="B11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s" s="20">
-        <v>101</v>
+      <c r="C11" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" ht="30" customHeight="1">
-      <c r="A12" t="s" s="4">
+    <row r="12" spans="1:5" ht="30" customHeight="1">
+      <c r="A12" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B12" t="s" s="4">
+      <c r="C12" s="20" t="s">
         <v>103</v>
-      </c>
-      <c r="C12" t="s" s="20">
-        <v>104</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" ht="45" customHeight="1">
-      <c r="A13" t="s" s="4">
+    <row r="13" spans="1:5" ht="45" customHeight="1">
+      <c r="A13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B13" t="s" s="4">
+      <c r="C13" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="C13" t="s" s="20">
-        <v>107</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" ht="30" customHeight="1">
-      <c r="A14" t="s" s="4">
+    <row r="14" spans="1:5" ht="30" customHeight="1">
+      <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s" s="4">
+      <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s" s="20">
+      <c r="C14" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="A15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>108</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="4">
-        <v>49</v>
-      </c>
-      <c r="B15" t="s" s="4">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s" s="20">
-        <v>109</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="4">
+    <row r="16" spans="1:5" ht="15" customHeight="1">
+      <c r="A16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B16" t="s" s="4">
+      <c r="C16" s="20" t="s">
         <v>111</v>
-      </c>
-      <c r="C16" t="s" s="20">
-        <v>112</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" ht="30" customHeight="1">
-      <c r="A17" t="s" s="4">
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B17" t="s" s="4">
+      <c r="C17" s="20" t="s">
         <v>114</v>
-      </c>
-      <c r="C17" t="s" s="20">
-        <v>115</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="4">
+    <row r="18" spans="1:5" ht="15" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B18" t="s" s="4">
+      <c r="C18" s="20" t="s">
         <v>117</v>
-      </c>
-      <c r="C18" t="s" s="20">
-        <v>118</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="4">
+    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="A19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s" s="4">
+      <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s" s="20">
-        <v>119</v>
+      <c r="C19" s="20" t="s">
+        <v>118</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="4">
+    <row r="20" spans="1:5" ht="15" customHeight="1">
+      <c r="A20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s" s="4">
+      <c r="B20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C20" t="s" s="20">
-        <v>120</v>
+      <c r="C20" s="20" t="s">
+        <v>119</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
-      <c r="A21" t="s" s="4">
+    <row r="21" spans="1:5" ht="15" customHeight="1">
+      <c r="A21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s" s="4">
+      <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C21" t="s" s="20">
-        <v>121</v>
+      <c r="C21" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" ht="30" customHeight="1">
-      <c r="A22" t="s" s="4">
+    <row r="22" spans="1:5" ht="30" customHeight="1">
+      <c r="A22" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B22" t="s" s="4">
+      <c r="B22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C22" t="s" s="20">
+      <c r="C22" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" ht="30" customHeight="1">
-      <c r="A23" t="s" s="4">
-        <v>59</v>
-      </c>
-      <c r="B23" t="s" s="4">
-        <v>60</v>
-      </c>
-      <c r="C23" t="s" s="20">
+      <c r="D23" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="30" customHeight="1">
+      <c r="A24" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" ht="30" customHeight="1">
-      <c r="A24" t="s" s="4">
+      <c r="B24" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B24" t="s" s="4">
+      <c r="C24" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="C24" t="s" s="20">
-        <v>126</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" ht="45" customHeight="1">
-      <c r="A25" t="s" s="4">
+    <row r="25" spans="1:5" ht="45" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B25" t="s" s="4">
+      <c r="C25" s="20" t="s">
         <v>128</v>
-      </c>
-      <c r="C25" t="s" s="20">
-        <v>129</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" ht="30" customHeight="1">
-      <c r="A26" t="s" s="4">
+    <row r="26" spans="1:5" ht="30" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s" s="4">
+      <c r="B26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C26" t="s" s="20">
-        <v>130</v>
+      <c r="C26" s="20" t="s">
+        <v>129</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" ht="75" customHeight="1">
-      <c r="A27" t="s" s="4">
+    <row r="27" spans="1:5" ht="75" customHeight="1">
+      <c r="A27" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B27" t="s" s="4">
+      <c r="C27" s="20" t="s">
         <v>132</v>
-      </c>
-      <c r="C27" t="s" s="20">
-        <v>133</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" ht="15" customHeight="1">
-      <c r="A28" t="s" s="4">
+    <row r="28" spans="1:5" ht="15" customHeight="1">
+      <c r="A28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B28" t="s" s="4">
+      <c r="B28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C28" t="s" s="20">
-        <v>134</v>
+      <c r="C28" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" ht="15" customHeight="1">
-      <c r="A29" t="s" s="4">
+    <row r="29" spans="1:5" ht="15" customHeight="1">
+      <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B29" t="s" s="4">
+      <c r="B29" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C29" t="s" s="20">
-        <v>135</v>
+      <c r="C29" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" ht="15" customHeight="1">
-      <c r="A30" t="s" s="4">
+    <row r="30" spans="1:5" ht="15" customHeight="1">
+      <c r="A30" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B30" t="s" s="4">
+      <c r="C30" s="20" t="s">
         <v>137</v>
-      </c>
-      <c r="C30" t="s" s="20">
-        <v>138</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" ht="15" customHeight="1">
-      <c r="A31" t="s" s="4">
+    <row r="31" spans="1:5" ht="15" customHeight="1">
+      <c r="A31" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B31" t="s" s="4">
+      <c r="B31" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s" s="20">
-        <v>139</v>
+      <c r="C31" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" ht="30" customHeight="1">
-      <c r="A32" t="s" s="4">
+    <row r="32" spans="1:5" ht="30" customHeight="1">
+      <c r="A32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B32" t="s" s="4">
+      <c r="C32" s="20" t="s">
         <v>141</v>
-      </c>
-      <c r="C32" t="s" s="20">
-        <v>142</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" ht="15" customHeight="1">
-      <c r="A33" t="s" s="4">
+    <row r="33" spans="1:5" ht="15" customHeight="1">
+      <c r="A33" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B33" t="s" s="4">
+      <c r="C33" s="20" t="s">
         <v>144</v>
-      </c>
-      <c r="C33" t="s" s="20">
-        <v>145</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" ht="30" customHeight="1">
-      <c r="A34" t="s" s="4">
+    <row r="34" spans="1:5" ht="30" customHeight="1">
+      <c r="A34" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B34" t="s" s="4">
+      <c r="C34" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="C34" t="s" s="20">
-        <v>148</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" ht="30" customHeight="1">
-      <c r="A35" t="s" s="4">
+    <row r="35" spans="1:5" ht="30" customHeight="1">
+      <c r="A35" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B35" t="s" s="4">
+      <c r="C35" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="C35" t="s" s="20">
-        <v>151</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" ht="30" customHeight="1">
-      <c r="A36" t="s" s="4">
+    <row r="36" spans="1:5" ht="30" customHeight="1">
+      <c r="A36" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B36" t="s" s="4">
+      <c r="B36" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C36" t="s" s="20">
-        <v>152</v>
+      <c r="C36" s="20" t="s">
+        <v>151</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" ht="30" customHeight="1">
-      <c r="A37" t="s" s="4">
+    <row r="37" spans="1:5" ht="30" customHeight="1">
+      <c r="A37" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B37" t="s" s="4">
+      <c r="C37" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="C37" t="s" s="20">
-        <v>155</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" ht="30" customHeight="1">
-      <c r="A38" t="s" s="4">
+    <row r="38" spans="1:5" ht="30" customHeight="1">
+      <c r="A38" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B38" t="s" s="4">
+      <c r="C38" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="C38" t="s" s="20">
-        <v>158</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" ht="30" customHeight="1">
-      <c r="A39" t="s" s="4">
+    <row r="39" spans="1:5" ht="30" customHeight="1">
+      <c r="A39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B39" t="s" s="4">
+      <c r="B39" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C39" t="s" s="20">
-        <v>159</v>
+      <c r="C39" s="20" t="s">
+        <v>158</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" ht="30" customHeight="1">
-      <c r="A40" t="s" s="4">
+    <row r="40" spans="1:5" ht="30" customHeight="1">
+      <c r="A40" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B40" t="s" s="4">
+      <c r="C40" s="20" t="s">
         <v>161</v>
-      </c>
-      <c r="C40" t="s" s="20">
-        <v>162</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" ht="30" customHeight="1">
-      <c r="A41" t="s" s="4">
+    <row r="41" spans="1:5" ht="30" customHeight="1">
+      <c r="A41" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B41" t="s" s="4">
+      <c r="C41" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="C41" t="s" s="20">
-        <v>165</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" ht="30" customHeight="1">
-      <c r="A42" t="s" s="4">
+    <row r="42" spans="1:5" ht="30" customHeight="1">
+      <c r="A42" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B42" t="s" s="4">
+      <c r="C42" s="20" t="s">
         <v>167</v>
-      </c>
-      <c r="C42" t="s" s="20">
-        <v>168</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" ht="30" customHeight="1">
-      <c r="A43" t="s" s="4">
+    <row r="43" spans="1:5" ht="30" customHeight="1">
+      <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B43" t="s" s="4">
+      <c r="B43" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C43" t="s" s="20">
-        <v>169</v>
+      <c r="C43" s="20" t="s">
+        <v>168</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edited team report and README
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,32 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezhil\Documents\agile\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" r:id="rId1"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
-    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
-    <sheet name="Stories" sheetId="8" r:id="rId8"/>
+    <sheet name="Team" sheetId="1" r:id="rId4"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId5"/>
+    <sheet name="Burndown" sheetId="3" r:id="rId6"/>
+    <sheet name="Sprint1" sheetId="4" r:id="rId7"/>
+    <sheet name="Sprint2" sheetId="5" r:id="rId8"/>
+    <sheet name="Sprint3" sheetId="6" r:id="rId9"/>
+    <sheet name="Sprint4" sheetId="7" r:id="rId10"/>
+    <sheet name="Stories" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="172">
   <si>
     <t>Initials</t>
   </si>
@@ -93,7 +86,7 @@
   <si>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color indexed="11"/>
         <rFont val="Verdana"/>
@@ -260,6 +253,7 @@
   <si>
     <t>Reject illegitimate dates</t>
   </si>
+  <si/>
   <si>
     <t>Date</t>
   </si>
@@ -306,6 +300,12 @@
     <t>Avoid:</t>
   </si>
   <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t>Story Description</t>
   </si>
   <si>
@@ -541,39 +541,59 @@
   </si>
   <si>
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
-  </si>
-  <si>
-    <t>pending</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="m/d"/>
+    <numFmt numFmtId="60" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
@@ -620,36 +640,63 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -660,89 +707,29 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF878787"/>
-      <rgbColor rgb="FF4A7DBB"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ff888888"/>
+      <rgbColor rgb="ff4a7ebb"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -751,10 +738,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.3600800000000003E-2"/>
-          <c:y val="5.9319799999999999E-2"/>
-          <c:w val="0.91139899999999996"/>
-          <c:h val="0.83215899999999998"/>
+          <c:x val="0.0836458"/>
+          <c:y val="0.0600707"/>
+          <c:w val="0.911354"/>
+          <c:h val="0.830193"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -767,6 +754,9 @@
             <c:v>Series1</c:v>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln w="28575" cap="flat">
               <a:solidFill>
                 <a:srgbClr val="4A7EBB"/>
@@ -778,7 +768,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="6"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -793,64 +783,85 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
+            <c:strRef>
+              <c:f>'Burndown'!$A$2:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40947</c:v>
+                  <c:v>2/9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40961</c:v>
+                  <c:v>2/23</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>'Burndown'!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F9B3-458A-8575-91B623E9171A}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
         <c:axId val="2094734552"/>
         <c:axId val="2094734553"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2094734552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -868,22 +879,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2094734553"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:lblAlgn val="ctr"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2094734553"/>
         <c:scaling>
@@ -920,14 +930,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2094734552"/>
@@ -949,7 +958,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -964,41 +972,36 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>510979</xdr:colOff>
+      <xdr:colOff>510978</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>550</xdr:rowOff>
+      <xdr:rowOff>549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>111642</xdr:colOff>
+      <xdr:colOff>109574</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>126732</xdr:rowOff>
+      <xdr:rowOff>97293</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="1323778" y="1715049"/>
+        <a:ext cx="3840397" cy="2325595"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1008,7 +1011,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1134,7 +1137,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1143,7 +1146,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1152,9 +1155,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1226,7 +1229,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1234,7 +1237,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1253,7 +1256,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1262,10 +1265,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1283,7 +1286,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1309,7 +1312,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1335,7 +1338,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1361,7 +1364,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1387,7 +1390,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1413,7 +1416,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1439,7 +1442,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1465,7 +1468,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1491,7 +1494,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1504,15 +1507,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1527,15 +1524,15 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1554,7 +1551,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1580,7 +1577,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1606,7 +1603,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1632,7 +1629,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1658,7 +1655,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1684,7 +1681,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1710,7 +1707,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1736,7 +1733,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1762,7 +1759,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1788,7 +1785,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1801,15 +1798,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1823,7 +1814,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1842,7 +1833,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1851,10 +1842,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1872,7 +1863,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1898,7 +1889,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1924,7 +1915,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1950,7 +1941,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1976,7 +1967,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2002,7 +1993,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2028,7 +2019,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2054,7 +2045,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2080,7 +2071,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2093,147 +2084,140 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.3046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3828125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.35156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.15234375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
     <col min="6" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2242,7 +2226,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2250,321 +2234,321 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV25"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.3046875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.69140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.4609375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="6.69140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.69140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.35156" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.67188" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.67188" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.67188" style="5" customWidth="1"/>
     <col min="6" max="256" width="11" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s" s="4">
         <v>28</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>34</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s" s="4">
         <v>36</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>37</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s" s="4">
         <v>38</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s" s="4">
         <v>42</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s" s="4">
         <v>44</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s" s="4">
         <v>46</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+    <row r="12" ht="15" customHeight="1">
+      <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s" s="4">
         <v>49</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s" s="4">
         <v>50</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s" s="4">
         <v>52</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s" s="4">
         <v>54</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s" s="4">
         <v>55</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s" s="4">
         <v>56</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s" s="4">
         <v>62</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s" s="4">
         <v>64</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s" s="4">
         <v>66</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="3"/>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s" s="4">
         <v>67</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s" s="4">
         <v>68</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s" s="4">
         <v>69</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s" s="4">
         <v>70</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="3"/>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" t="s" s="4">
         <v>72</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" ht="15" customHeight="1">
       <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s" s="4">
         <v>73</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" t="s" s="4">
         <v>74</v>
       </c>
       <c r="D25" s="3"/>
@@ -2572,7 +2556,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2580,291 +2564,292 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV26"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.69140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="7" customWidth="1"/>
-    <col min="7" max="256" width="11" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.6719" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="7.17188" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.85156" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11" style="6" customWidth="1"/>
+    <col min="8" max="256" width="11" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" ht="13.5" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>80</v>
       </c>
+      <c r="F1" t="s" s="2">
+        <v>81</v>
+      </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+    <row r="2" ht="13.5" customHeight="1">
+      <c r="A2" s="7">
         <v>40947</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>24</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="6">
+      <c r="D2" s="3">
         <v>0</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="9"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" s="7">
         <v>40961</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>18</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <f>B2-B3</f>
         <v>6</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>250</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <v>120</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>125</v>
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+    <row r="5" ht="13.5" customHeight="1">
+      <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+    <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+    <row r="7" ht="13.5" customHeight="1">
+      <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+    <row r="8" ht="13.5" customHeight="1">
+      <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+    <row r="9" ht="13.5" customHeight="1">
+      <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="9"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+    <row r="10" ht="13.5" customHeight="1">
+      <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+    <row r="11" ht="13.5" customHeight="1">
+      <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+    <row r="12" ht="13.5" customHeight="1">
+      <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+    <row r="13" ht="13.5" customHeight="1">
+      <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="9"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+    <row r="14" ht="13.5" customHeight="1">
+      <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="9"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+    <row r="15" ht="13.5" customHeight="1">
+      <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="9"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+    <row r="16" ht="13.5" customHeight="1">
+      <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="9"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
+    <row r="17" ht="13.5" customHeight="1">
+      <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
+    <row r="18" ht="13.5" customHeight="1">
+      <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
+    <row r="19" ht="13.5" customHeight="1">
+      <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="9"/>
+      <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+    <row r="20" ht="13.5" customHeight="1">
+      <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="9"/>
+      <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
+    <row r="21" ht="13.5" customHeight="1">
+      <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
+    <row r="22" ht="13.5" customHeight="1">
+      <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="9"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
+    <row r="23" ht="13.5" customHeight="1">
+      <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="9"/>
+      <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
+    <row r="24" ht="13.5" customHeight="1">
+      <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="9"/>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+    <row r="25" ht="13.5" customHeight="1">
+      <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="9"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+    <row r="26" ht="13.5" customHeight="1">
+      <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="9"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2873,275 +2858,275 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV19"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.69140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="24.4609375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="6.69140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="11" style="11" customWidth="1"/>
-    <col min="5" max="5" width="10.3046875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="10.3828125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="8.4609375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.3046875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="10.69140625" style="11" customWidth="1"/>
-    <col min="10" max="256" width="11" style="11" customWidth="1"/>
+    <col min="1" max="1" width="7.67188" style="9" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.67188" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.3516" style="9" customWidth="1"/>
+    <col min="6" max="6" width="10.3516" style="9" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="9.35156" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.6719" style="9" customWidth="1"/>
+    <col min="10" max="256" width="11" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="E1" t="s" s="11">
         <v>82</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" t="s" s="11">
         <v>83</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" t="s" s="11">
         <v>84</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" t="s" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="I1" t="s" s="11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s" s="4">
         <v>10</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="6">
+      <c r="E2" s="3">
         <v>7</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="3">
         <v>45</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="3">
         <v>5</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="3">
         <v>30</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="I2" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>15</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <v>3</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="3">
         <v>30</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="3">
         <v>7</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="3">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="I3" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>10</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>5</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="3">
         <v>60</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="3">
         <v>5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="3">
         <v>60</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="I4" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>15</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>10</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <v>45</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="3">
         <v>15</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="3">
         <v>40</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="I5" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <v>5</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="3">
         <v>20</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="3">
         <v>20</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="3">
         <v>60</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="I6" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <v>5</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="3">
         <v>20</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="3">
         <v>20</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="3">
         <v>5</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="15"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="15"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="15"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="15"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="15"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="12" t="s">
-        <v>87</v>
+      <c r="B13" t="s" s="10">
+        <v>88</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3149,23 +3134,23 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="12"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="3"/>
-      <c r="B15" s="12" t="s">
-        <v>88</v>
+      <c r="B15" t="s" s="10">
+        <v>89</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -3173,45 +3158,45 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" s="15"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="3"/>
-      <c r="B18" s="15"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="3"/>
-      <c r="B19" s="12" t="s">
-        <v>89</v>
+      <c r="B19" t="s" s="10">
+        <v>90</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -3219,11 +3204,11 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3231,61 +3216,66 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="16" customWidth="1"/>
-    <col min="2" max="2" width="24.69140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="256" width="11" style="16" customWidth="1"/>
+    <col min="1" max="1" width="11" style="13" customWidth="1"/>
+    <col min="2" max="2" width="24.6719" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11" style="13" customWidth="1"/>
+    <col min="4" max="4" width="11" style="13" customWidth="1"/>
+    <col min="5" max="5" width="11" style="13" customWidth="1"/>
+    <col min="6" max="6" width="11" style="13" customWidth="1"/>
+    <col min="7" max="7" width="11" style="13" customWidth="1"/>
+    <col min="8" max="8" width="11" style="13" customWidth="1"/>
+    <col min="9" max="9" width="11" style="13" customWidth="1"/>
+    <col min="10" max="256" width="11" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="E1" t="s" s="11">
         <v>82</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" t="s" s="11">
         <v>83</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" t="s" s="11">
         <v>84</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" t="s" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="I1" t="s" s="11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>169</v>
+      <c r="D2" t="s" s="4">
+        <v>91</v>
       </c>
       <c r="E2" s="3">
         <v>12</v>
@@ -3297,18 +3287,18 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>169</v>
+      <c r="D3" t="s" s="4">
+        <v>91</v>
       </c>
       <c r="E3" s="3">
         <v>15</v>
@@ -3320,18 +3310,18 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>169</v>
+      <c r="D4" t="s" s="4">
+        <v>92</v>
       </c>
       <c r="E4" s="3">
         <v>5</v>
@@ -3339,22 +3329,26 @@
       <c r="F4" s="3">
         <v>45</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="3">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3">
+        <v>48</v>
+      </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>169</v>
+      <c r="D5" t="s" s="4">
+        <v>92</v>
       </c>
       <c r="E5" s="3">
         <v>20</v>
@@ -3362,22 +3356,26 @@
       <c r="F5" s="3">
         <v>60</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="3">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3">
+        <v>30</v>
+      </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s" s="4">
         <v>64</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>170</v>
+      <c r="D6" t="s" s="4">
+        <v>92</v>
       </c>
       <c r="E6" s="3">
         <v>20</v>
@@ -3393,18 +3391,18 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>170</v>
+      <c r="D7" t="s" s="4">
+        <v>92</v>
       </c>
       <c r="E7" s="3">
         <v>7</v>
@@ -3420,7 +3418,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3431,7 +3429,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3442,7 +3440,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3455,7 +3453,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3463,46 +3461,55 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="256" width="11" style="17" customWidth="1"/>
+    <col min="1" max="1" width="11" style="14" customWidth="1"/>
+    <col min="2" max="2" width="11" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11" style="14" customWidth="1"/>
+    <col min="4" max="4" width="11" style="14" customWidth="1"/>
+    <col min="5" max="5" width="11" style="14" customWidth="1"/>
+    <col min="6" max="6" width="11" style="14" customWidth="1"/>
+    <col min="7" max="7" width="11" style="14" customWidth="1"/>
+    <col min="8" max="8" width="11" style="14" customWidth="1"/>
+    <col min="9" max="9" width="11" style="14" customWidth="1"/>
+    <col min="10" max="256" width="11" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="E1" t="s" s="11">
         <v>82</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" t="s" s="11">
         <v>83</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" t="s" s="11">
         <v>84</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" t="s" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" t="s" s="11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3513,7 +3520,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3524,7 +3531,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3535,7 +3542,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3546,7 +3553,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3557,7 +3564,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3568,7 +3575,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3579,7 +3586,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3590,7 +3597,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3603,7 +3610,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3611,46 +3618,55 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="256" width="11" style="18" customWidth="1"/>
+    <col min="1" max="1" width="11" style="15" customWidth="1"/>
+    <col min="2" max="2" width="11" style="15" customWidth="1"/>
+    <col min="3" max="3" width="11" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11" style="15" customWidth="1"/>
+    <col min="7" max="7" width="11" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11" style="15" customWidth="1"/>
+    <col min="9" max="9" width="11" style="15" customWidth="1"/>
+    <col min="10" max="256" width="11" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="E1" t="s" s="11">
         <v>82</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" t="s" s="11">
         <v>83</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" t="s" s="11">
         <v>84</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" t="s" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" t="s" s="11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3661,7 +3677,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3672,7 +3688,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3683,7 +3699,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3694,7 +3710,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3705,7 +3721,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3716,7 +3732,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3727,7 +3743,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3738,7 +3754,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3751,7 +3767,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3759,581 +3775,583 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV43"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="19" customWidth="1"/>
-    <col min="2" max="2" width="24.4609375" style="19" customWidth="1"/>
-    <col min="3" max="3" width="49.3828125" style="19" customWidth="1"/>
-    <col min="4" max="256" width="11" style="19" customWidth="1"/>
+    <col min="1" max="1" width="11" style="16" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="16" customWidth="1"/>
+    <col min="3" max="3" width="49.3516" style="16" customWidth="1"/>
+    <col min="4" max="4" width="11" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11" style="16" customWidth="1"/>
+    <col min="6" max="256" width="11" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>90</v>
+      <c r="C1" t="s" s="10">
+        <v>93</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>91</v>
+      <c r="C2" t="s" s="17">
+        <v>94</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>92</v>
+      <c r="C3" t="s" s="17">
+        <v>95</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>93</v>
+      <c r="C4" t="s" s="17">
+        <v>96</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>34</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>94</v>
+      <c r="C5" t="s" s="17">
+        <v>97</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>36</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>95</v>
+      <c r="C6" t="s" s="17">
+        <v>98</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>37</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>38</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>96</v>
+      <c r="C7" t="s" s="17">
+        <v>99</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" ht="45" customHeight="1">
+      <c r="A8" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>97</v>
+      <c r="C8" t="s" s="17">
+        <v>100</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>98</v>
+      <c r="C9" t="s" s="17">
+        <v>101</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>99</v>
+      <c r="C10" t="s" s="17">
+        <v>102</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s" s="4">
         <v>46</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>100</v>
+      <c r="C11" t="s" s="17">
+        <v>103</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>103</v>
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" t="s" s="4">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s" s="4">
+        <v>105</v>
+      </c>
+      <c r="C12" t="s" s="17">
+        <v>106</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>106</v>
+    <row r="13" ht="45" customHeight="1">
+      <c r="A13" t="s" s="4">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s" s="4">
+        <v>108</v>
+      </c>
+      <c r="C13" t="s" s="17">
+        <v>109</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>107</v>
+      <c r="C14" t="s" s="17">
+        <v>110</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" t="s" s="4">
         <v>49</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s" s="4">
         <v>50</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>108</v>
+      <c r="C15" t="s" s="17">
+        <v>111</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>111</v>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" t="s" s="4">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s" s="4">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s" s="17">
+        <v>114</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>114</v>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" t="s" s="4">
+        <v>115</v>
+      </c>
+      <c r="B17" t="s" s="4">
+        <v>116</v>
+      </c>
+      <c r="C17" t="s" s="17">
+        <v>117</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>117</v>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="s" s="4">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s" s="4">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s" s="17">
+        <v>120</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>118</v>
+      <c r="C19" t="s" s="17">
+        <v>121</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>119</v>
+      <c r="C20" t="s" s="17">
+        <v>122</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" t="s" s="4">
         <v>55</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s" s="4">
         <v>56</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>120</v>
+      <c r="C21" t="s" s="17">
+        <v>123</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="22" ht="30" customHeight="1">
+      <c r="A22" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>121</v>
+      <c r="C22" t="s" s="17">
+        <v>124</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="23" ht="30" customHeight="1">
+      <c r="A23" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="C23" s="20" t="s">
-        <v>122</v>
+      <c r="C23" t="s" s="17">
+        <v>125</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>125</v>
+    <row r="24" ht="30" customHeight="1">
+      <c r="A24" t="s" s="4">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s" s="4">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s" s="17">
+        <v>128</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>128</v>
+    <row r="25" ht="45" customHeight="1">
+      <c r="A25" t="s" s="4">
+        <v>129</v>
+      </c>
+      <c r="B25" t="s" s="4">
+        <v>130</v>
+      </c>
+      <c r="C25" t="s" s="17">
+        <v>131</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="26" ht="30" customHeight="1">
+      <c r="A26" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>129</v>
+      <c r="C26" t="s" s="17">
+        <v>132</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>132</v>
+    <row r="27" ht="75" customHeight="1">
+      <c r="A27" t="s" s="4">
+        <v>133</v>
+      </c>
+      <c r="B27" t="s" s="4">
+        <v>134</v>
+      </c>
+      <c r="C27" t="s" s="17">
+        <v>135</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s" s="4">
         <v>64</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>133</v>
+      <c r="C28" t="s" s="17">
+        <v>136</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>134</v>
+      <c r="C29" t="s" s="17">
+        <v>137</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>137</v>
+    <row r="30" ht="15" customHeight="1">
+      <c r="A30" t="s" s="4">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s" s="4">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s" s="17">
+        <v>140</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" t="s" s="4">
         <v>67</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s" s="4">
         <v>68</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>138</v>
+      <c r="C31" t="s" s="17">
+        <v>141</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>141</v>
+    <row r="32" ht="30" customHeight="1">
+      <c r="A32" t="s" s="4">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s" s="4">
+        <v>143</v>
+      </c>
+      <c r="C32" t="s" s="17">
+        <v>144</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>144</v>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" t="s" s="4">
+        <v>145</v>
+      </c>
+      <c r="B33" t="s" s="4">
+        <v>146</v>
+      </c>
+      <c r="C33" t="s" s="17">
+        <v>147</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>147</v>
+    <row r="34" ht="30" customHeight="1">
+      <c r="A34" t="s" s="4">
+        <v>148</v>
+      </c>
+      <c r="B34" t="s" s="4">
+        <v>149</v>
+      </c>
+      <c r="C34" t="s" s="17">
+        <v>150</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>150</v>
+    <row r="35" ht="30" customHeight="1">
+      <c r="A35" t="s" s="4">
+        <v>151</v>
+      </c>
+      <c r="B35" t="s" s="4">
+        <v>152</v>
+      </c>
+      <c r="C35" t="s" s="17">
+        <v>153</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+    <row r="36" ht="30" customHeight="1">
+      <c r="A36" t="s" s="4">
         <v>69</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s" s="4">
         <v>70</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>151</v>
+      <c r="C36" t="s" s="17">
+        <v>154</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>154</v>
+    <row r="37" ht="30" customHeight="1">
+      <c r="A37" t="s" s="4">
+        <v>155</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>156</v>
+      </c>
+      <c r="C37" t="s" s="17">
+        <v>157</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>157</v>
+    <row r="38" ht="30" customHeight="1">
+      <c r="A38" t="s" s="4">
+        <v>158</v>
+      </c>
+      <c r="B38" t="s" s="4">
+        <v>159</v>
+      </c>
+      <c r="C38" t="s" s="17">
+        <v>160</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+    <row r="39" ht="30" customHeight="1">
+      <c r="A39" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="C39" s="20" t="s">
-        <v>158</v>
+      <c r="C39" t="s" s="17">
+        <v>161</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>161</v>
+    <row r="40" ht="30" customHeight="1">
+      <c r="A40" t="s" s="4">
+        <v>162</v>
+      </c>
+      <c r="B40" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C40" t="s" s="17">
+        <v>164</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>164</v>
+    <row r="41" ht="30" customHeight="1">
+      <c r="A41" t="s" s="4">
+        <v>165</v>
+      </c>
+      <c r="B41" t="s" s="4">
+        <v>166</v>
+      </c>
+      <c r="C41" t="s" s="17">
+        <v>167</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>167</v>
+    <row r="42" ht="30" customHeight="1">
+      <c r="A42" t="s" s="4">
+        <v>168</v>
+      </c>
+      <c r="B42" t="s" s="4">
+        <v>169</v>
+      </c>
+      <c r="C42" t="s" s="17">
+        <v>170</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+    <row r="43" ht="30" customHeight="1">
+      <c r="A43" t="s" s="4">
         <v>73</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>168</v>
+      <c r="C43" t="s" s="17">
+        <v>171</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
updated the team report
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,32 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
-  <workbookPr date1904="1" autoCompressPictures="0"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" r:id="rId1"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
-    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
-    <sheet name="Stories" sheetId="8" r:id="rId8"/>
+    <sheet name="Team" sheetId="1" r:id="rId4"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId5"/>
+    <sheet name="Burndown" sheetId="3" r:id="rId6"/>
+    <sheet name="Sprint1" sheetId="4" r:id="rId7"/>
+    <sheet name="Sprint2" sheetId="5" r:id="rId8"/>
+    <sheet name="Sprint3" sheetId="6" r:id="rId9"/>
+    <sheet name="Sprint4" sheetId="7" r:id="rId10"/>
+    <sheet name="Stories" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="173">
   <si>
     <t>Initials</t>
   </si>
@@ -93,7 +86,7 @@
   <si>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color indexed="11"/>
         <rFont val="Verdana"/>
@@ -260,6 +253,7 @@
   <si>
     <t>Reject illegitimate dates</t>
   </si>
+  <si/>
   <si>
     <t>Date</t>
   </si>
@@ -306,6 +300,9 @@
     <t>Avoid:</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
     <t>pending</t>
   </si>
   <si>
@@ -547,53 +544,64 @@
   </si>
   <si>
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
-  </si>
-  <si>
-    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="m/d"/>
+    <numFmt numFmtId="60" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Verdana"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Cambria"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="11"/>
-      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="3">
@@ -634,133 +642,91 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="13">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF888888"/>
-      <rgbColor rgb="FF4A7EBB"/>
-      <rgbColor rgb="00F20884"/>
-      <rgbColor rgb="0000ABEA"/>
-      <rgbColor rgb="00900000"/>
-      <rgbColor rgb="00006411"/>
-      <rgbColor rgb="00000090"/>
-      <rgbColor rgb="0090713A"/>
-      <rgbColor rgb="004600A5"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ff888888"/>
+      <rgbColor rgb="ff4a7ebb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -769,9 +735,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="18"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -780,10 +744,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0836458"/>
-          <c:y val="0.0600707"/>
-          <c:w val="0.911354"/>
-          <c:h val="0.830193"/>
+          <c:x val="0.0836907"/>
+          <c:y val="0.0608311"/>
+          <c:w val="0.911309"/>
+          <c:h val="0.828202"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -796,6 +760,9 @@
             <c:v>Series1</c:v>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln w="28575" cap="flat">
               <a:solidFill>
                 <a:srgbClr val="4A7EBB"/>
@@ -807,7 +774,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -822,65 +789,88 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
+            <c:strRef>
+              <c:f>'Burndown'!$A$2:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40947.0</c:v>
+                  <c:v>2/9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40961.0</c:v>
+                  <c:v>2/23</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="d\-mmm">
-                  <c:v>40982.0</c:v>
+                <c:pt idx="2">
+                  <c:v>15-Mar</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>'Burndown'!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18.000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0</c:v>
+                  <c:v>13.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2107830952"/>
-        <c:axId val="2107827928"/>
+        <c:axId val="2094734552"/>
+        <c:axId val="2094734553"/>
       </c:lineChart>
-      <c:dateAx>
-        <c:axId val="2107830952"/>
+      <c:catAx>
+        <c:axId val="2094734552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -898,24 +888,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107827928"/>
+        <c:crossAx val="2094734553"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:lblAlgn val="ctr"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="2107827928"/>
+        <c:axId val="2094734553"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -950,21 +939,20 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107830952"/>
+        <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="6.0"/>
-        <c:minorUnit val="3.0"/>
+        <c:majorUnit val="6"/>
+        <c:minorUnit val="3"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -979,7 +967,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -994,41 +981,36 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>510978</xdr:colOff>
+      <xdr:colOff>510977</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>109574</xdr:colOff>
+      <xdr:colOff>107516</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>97293</xdr:rowOff>
+      <xdr:rowOff>68222</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="1323777" y="1715049"/>
+        <a:ext cx="3838340" cy="2296524"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1038,7 +1020,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1164,7 +1146,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1173,7 +1155,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1182,7 +1164,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1256,7 +1238,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1264,7 +1246,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1283,7 +1265,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1313,7 +1295,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1339,7 +1321,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1365,7 +1347,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1391,7 +1373,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1417,7 +1399,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1443,7 +1425,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1469,7 +1451,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1495,7 +1477,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1521,7 +1503,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1534,15 +1516,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1557,7 +1533,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1565,7 +1541,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1584,7 +1560,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1610,7 +1586,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1636,7 +1612,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1662,7 +1638,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1688,7 +1664,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1714,7 +1690,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1740,7 +1716,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1766,7 +1742,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1792,7 +1768,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1818,7 +1794,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1831,15 +1807,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1853,7 +1823,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1872,7 +1842,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1902,7 +1872,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1928,7 +1898,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1954,7 +1924,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1980,7 +1950,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2006,7 +1976,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2032,7 +2002,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2058,7 +2028,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2084,7 +2054,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2110,7 +2080,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2123,147 +2093,140 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.35156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
     <col min="6" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2272,384 +2235,377 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV25"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:D24"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.35156" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.67188" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.67188" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.67188" style="5" customWidth="1"/>
     <col min="6" max="256" width="11" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>34</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s" s="4">
         <v>36</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>37</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s" s="4">
         <v>38</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3">
         <v>3</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s" s="4">
         <v>46</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="3">
         <v>3</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s" s="4">
         <v>49</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s" s="4">
         <v>50</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="3">
         <v>2</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="3">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s" s="4">
         <v>55</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s" s="4">
         <v>56</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="3">
         <v>2</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="3">
         <v>2</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s" s="4">
         <v>64</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="3">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="3">
         <v>3</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s" s="4">
         <v>67</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s" s="4">
         <v>68</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s" s="4">
         <v>69</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s" s="4">
         <v>70</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="3">
         <v>3</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1">
+    <row r="25" ht="15" customHeight="1">
       <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s" s="4">
         <v>73</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" t="s" s="4">
         <v>74</v>
       </c>
       <c r="D25" s="3"/>
@@ -2657,59 +2613,53 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV26"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="6" customWidth="1"/>
-    <col min="7" max="256" width="11" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.6719" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="7.17188" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.85156" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11" style="6" customWidth="1"/>
+    <col min="8" max="256" width="11" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" ht="13.5" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>80</v>
       </c>
+      <c r="F1" t="s" s="2">
+        <v>81</v>
+      </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="13.5" customHeight="1">
+    <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="7">
         <v>40947</v>
       </c>
@@ -2724,7 +2674,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="13.5" customHeight="1">
+    <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="7">
         <v>40961</v>
       </c>
@@ -2743,12 +2693,12 @@
       </c>
       <c r="F3" s="8">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>125</v>
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A4" s="18">
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" s="9">
         <v>40982</v>
       </c>
       <c r="B4" s="3">
@@ -2765,11 +2715,11 @@
       </c>
       <c r="F4" s="8">
         <f>(D4-D3)/E4*60</f>
-        <v>76.599999999999994</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="13.5" customHeight="1">
+    <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2778,7 +2728,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="13.5" customHeight="1">
+    <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2787,7 +2737,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="13.5" customHeight="1">
+    <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2796,7 +2746,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="13.5" customHeight="1">
+    <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2805,7 +2755,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="13.5" customHeight="1">
+    <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2814,7 +2764,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="13.5" customHeight="1">
+    <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2823,7 +2773,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="13.5" customHeight="1">
+    <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2832,7 +2782,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="13.5" customHeight="1">
+    <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2841,7 +2791,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="13.5" customHeight="1">
+    <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2850,7 +2800,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="13.5" customHeight="1">
+    <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2859,7 +2809,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="13.5" customHeight="1">
+    <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2868,7 +2818,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="13.5" customHeight="1">
+    <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2877,7 +2827,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="13.5" customHeight="1">
+    <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2886,7 +2836,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="13.5" customHeight="1">
+    <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2895,7 +2845,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="13.5" customHeight="1">
+    <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2904,7 +2854,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1">
+    <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2913,7 +2863,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="13.5" customHeight="1">
+    <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2922,7 +2872,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="13.5" customHeight="1">
+    <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2931,7 +2881,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="13.5" customHeight="1">
+    <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2940,7 +2890,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="13.5" customHeight="1">
+    <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2949,7 +2899,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="13.5" customHeight="1">
+    <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2958,7 +2908,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="13.5" customHeight="1">
+    <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2969,75 +2919,71 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV19"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11" style="9" customWidth="1"/>
-    <col min="5" max="6" width="10.28515625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="9" customWidth="1"/>
-    <col min="10" max="256" width="11" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.67188" style="10" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="6.67188" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11" style="10" customWidth="1"/>
+    <col min="5" max="5" width="10.3516" style="10" customWidth="1"/>
+    <col min="6" max="6" width="10.3516" style="10" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="9.35156" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.6719" style="10" customWidth="1"/>
+    <col min="10" max="256" width="11" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" t="s" s="12">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="F1" t="s" s="12">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" t="s" s="12">
         <v>84</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="H1" t="s" s="12">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="I1" t="s" s="12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s" s="4">
         <v>10</v>
       </c>
       <c r="D2" s="3"/>
@@ -3053,18 +2999,18 @@
       <c r="H2" s="3">
         <v>30</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="I2" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>15</v>
       </c>
       <c r="D3" s="3"/>
@@ -3080,18 +3026,18 @@
       <c r="H3" s="3">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="I3" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>10</v>
       </c>
       <c r="D4" s="3"/>
@@ -3107,18 +3053,18 @@
       <c r="H4" s="3">
         <v>60</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="I4" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>15</v>
       </c>
       <c r="D5" s="3"/>
@@ -3134,18 +3080,18 @@
       <c r="H5" s="3">
         <v>40</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="I5" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D6" s="3"/>
@@ -3161,18 +3107,18 @@
       <c r="H6" s="3">
         <v>60</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="I6" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D7" s="3"/>
@@ -3188,13 +3134,13 @@
       <c r="H7" s="3">
         <v>5</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="I7" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="12"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -3203,9 +3149,9 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="12"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -3214,9 +3160,9 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="12"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -3225,9 +3171,9 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="12"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3236,9 +3182,9 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="12"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -3247,10 +3193,10 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="10" t="s">
-        <v>87</v>
+      <c r="B13" t="s" s="11">
+        <v>88</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3260,9 +3206,9 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -3271,10 +3217,10 @@
       <c r="H14" s="3"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="3"/>
-      <c r="B15" s="10" t="s">
-        <v>88</v>
+      <c r="B15" t="s" s="11">
+        <v>89</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -3284,9 +3230,9 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" s="12"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -3295,9 +3241,9 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="12"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -3306,9 +3252,9 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="3"/>
-      <c r="B18" s="12"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3317,10 +3263,10 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="3"/>
-      <c r="B19" s="10" t="s">
-        <v>89</v>
+      <c r="B19" t="s" s="11">
+        <v>90</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -3332,74 +3278,74 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="13" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="13" customWidth="1"/>
-    <col min="3" max="256" width="11" style="13" customWidth="1"/>
+    <col min="1" max="1" width="11" style="14" customWidth="1"/>
+    <col min="2" max="2" width="24.6719" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11" style="14" customWidth="1"/>
+    <col min="4" max="4" width="11" style="14" customWidth="1"/>
+    <col min="5" max="5" width="11" style="14" customWidth="1"/>
+    <col min="6" max="6" width="11" style="14" customWidth="1"/>
+    <col min="7" max="7" width="11" style="14" customWidth="1"/>
+    <col min="8" max="8" width="11" style="14" customWidth="1"/>
+    <col min="9" max="9" width="11" style="14" customWidth="1"/>
+    <col min="10" max="256" width="11" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" t="s" s="12">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="F1" t="s" s="12">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" t="s" s="12">
         <v>84</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="H1" t="s" s="12">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="I1" t="s" s="12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>171</v>
+      <c r="D2" t="s" s="4">
+        <v>91</v>
       </c>
       <c r="E2" s="3">
         <v>12</v>
@@ -3413,20 +3359,22 @@
       <c r="H2" s="3">
         <v>70</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="I2" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>90</v>
+      <c r="D3" t="s" s="4">
+        <v>92</v>
       </c>
       <c r="E3" s="3">
         <v>15</v>
@@ -3442,18 +3390,18 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>91</v>
+      <c r="D4" t="s" s="4">
+        <v>93</v>
       </c>
       <c r="E4" s="3">
         <v>5</v>
@@ -3467,20 +3415,22 @@
       <c r="H4" s="3">
         <v>48</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="I4" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>91</v>
+      <c r="D5" t="s" s="4">
+        <v>93</v>
       </c>
       <c r="E5" s="3">
         <v>20</v>
@@ -3494,20 +3444,22 @@
       <c r="H5" s="3">
         <v>30</v>
       </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="I5" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>64</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>91</v>
+      <c r="D6" t="s" s="4">
+        <v>93</v>
       </c>
       <c r="E6" s="3">
         <v>20</v>
@@ -3521,20 +3473,22 @@
       <c r="H6" s="3">
         <v>45</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="I6" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>91</v>
+      <c r="D7" t="s" s="4">
+        <v>93</v>
       </c>
       <c r="E7" s="3">
         <v>7</v>
@@ -3548,9 +3502,11 @@
       <c r="H7" s="3">
         <v>25</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="I7" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3561,7 +3517,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3572,7 +3528,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3585,70 +3541,70 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="14" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="256" width="11" style="14" customWidth="1"/>
+    <col min="1" max="1" width="11" style="15" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="15" customWidth="1"/>
+    <col min="3" max="3" width="11" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11" style="15" customWidth="1"/>
+    <col min="7" max="7" width="11" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11" style="15" customWidth="1"/>
+    <col min="9" max="9" width="11" style="15" customWidth="1"/>
+    <col min="10" max="256" width="11" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" t="s" s="12">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="F1" t="s" s="12">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" t="s" s="12">
         <v>84</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="H1" t="s" s="12">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="I1" t="s" s="12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s" s="4">
         <v>10</v>
       </c>
       <c r="D2" s="3"/>
@@ -3658,14 +3614,14 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s" s="4">
         <v>10</v>
       </c>
       <c r="D3" s="3"/>
@@ -3675,14 +3631,14 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>46</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D4" s="3"/>
@@ -3692,14 +3648,14 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>49</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>50</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D5" s="3"/>
@@ -3709,41 +3665,65 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="4" t="s">
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>67</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>68</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="D6" t="s" s="4">
+        <v>91</v>
+      </c>
+      <c r="E6" s="3">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="D7" t="s" s="4">
+        <v>91</v>
+      </c>
+      <c r="E7" s="3">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3754,7 +3734,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3765,7 +3745,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3778,59 +3758,63 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="256" width="11" style="15" customWidth="1"/>
+    <col min="1" max="1" width="11" style="16" customWidth="1"/>
+    <col min="2" max="2" width="11" style="16" customWidth="1"/>
+    <col min="3" max="3" width="11" style="16" customWidth="1"/>
+    <col min="4" max="4" width="11" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11" style="16" customWidth="1"/>
+    <col min="6" max="6" width="11" style="16" customWidth="1"/>
+    <col min="7" max="7" width="11" style="16" customWidth="1"/>
+    <col min="8" max="8" width="11" style="16" customWidth="1"/>
+    <col min="9" max="9" width="11" style="16" customWidth="1"/>
+    <col min="10" max="256" width="11" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" t="s" s="12">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="F1" t="s" s="12">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" t="s" s="12">
         <v>84</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="H1" t="s" s="12">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="I1" t="s" s="12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3841,7 +3825,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3852,7 +3836,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3863,7 +3847,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3874,7 +3858,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3885,7 +3869,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3896,7 +3880,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3907,7 +3891,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3918,7 +3902,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3931,601 +3915,593 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV43"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="16" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" style="16" customWidth="1"/>
-    <col min="4" max="256" width="11" style="16" customWidth="1"/>
+    <col min="1" max="1" width="11" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="17" customWidth="1"/>
+    <col min="3" max="3" width="49.3516" style="17" customWidth="1"/>
+    <col min="4" max="4" width="11" style="17" customWidth="1"/>
+    <col min="5" max="5" width="11" style="17" customWidth="1"/>
+    <col min="6" max="256" width="11" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>92</v>
+      <c r="C1" t="s" s="11">
+        <v>94</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>93</v>
+      <c r="C2" t="s" s="18">
+        <v>95</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>94</v>
+      <c r="C3" t="s" s="18">
+        <v>96</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>95</v>
+      <c r="C4" t="s" s="18">
+        <v>97</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>34</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>96</v>
+      <c r="C5" t="s" s="18">
+        <v>98</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="4" t="s">
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>36</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>97</v>
+      <c r="C6" t="s" s="18">
+        <v>99</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="4" t="s">
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>37</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>38</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>98</v>
+      <c r="C7" t="s" s="18">
+        <v>100</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="45" customHeight="1">
-      <c r="A8" s="4" t="s">
+    <row r="8" ht="45" customHeight="1">
+      <c r="A8" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>99</v>
+      <c r="C8" t="s" s="18">
+        <v>101</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1">
-      <c r="A9" s="4" t="s">
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>100</v>
+      <c r="C9" t="s" s="18">
+        <v>102</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
-      <c r="A10" s="4" t="s">
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>101</v>
+      <c r="C10" t="s" s="18">
+        <v>103</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1">
-      <c r="A11" s="4" t="s">
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s" s="4">
         <v>46</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>102</v>
+      <c r="C11" t="s" s="18">
+        <v>104</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="17" t="s">
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" t="s" s="4">
         <v>105</v>
+      </c>
+      <c r="B12" t="s" s="4">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s" s="18">
+        <v>107</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="45" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="17" t="s">
+    <row r="13" ht="45" customHeight="1">
+      <c r="A13" t="s" s="4">
         <v>108</v>
+      </c>
+      <c r="B13" t="s" s="4">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s" s="18">
+        <v>110</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1">
-      <c r="A14" s="4" t="s">
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>109</v>
+      <c r="C14" t="s" s="18">
+        <v>111</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15" s="4" t="s">
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" t="s" s="4">
         <v>49</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s" s="4">
         <v>50</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>110</v>
+      <c r="C15" t="s" s="18">
+        <v>112</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="17" t="s">
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" t="s" s="4">
         <v>113</v>
+      </c>
+      <c r="B16" t="s" s="4">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s" s="18">
+        <v>115</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="17" t="s">
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" t="s" s="4">
         <v>116</v>
+      </c>
+      <c r="B17" t="s" s="4">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s" s="18">
+        <v>118</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="17" t="s">
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="s" s="4">
         <v>119</v>
+      </c>
+      <c r="B18" t="s" s="4">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s" s="18">
+        <v>121</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
-      <c r="A19" s="4" t="s">
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>120</v>
+      <c r="C19" t="s" s="18">
+        <v>122</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
-      <c r="A20" s="4" t="s">
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>121</v>
+      <c r="C20" t="s" s="18">
+        <v>123</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="4" t="s">
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" t="s" s="4">
         <v>55</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s" s="4">
         <v>56</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>122</v>
+      <c r="C21" t="s" s="18">
+        <v>124</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1">
-      <c r="A22" s="4" t="s">
+    <row r="22" ht="30" customHeight="1">
+      <c r="A22" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>123</v>
+      <c r="C22" t="s" s="18">
+        <v>125</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="4" t="s">
+    <row r="23" ht="30" customHeight="1">
+      <c r="A23" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>124</v>
+      <c r="C23" t="s" s="18">
+        <v>126</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="30" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="17" t="s">
+    <row r="24" ht="30" customHeight="1">
+      <c r="A24" t="s" s="4">
         <v>127</v>
+      </c>
+      <c r="B24" t="s" s="4">
+        <v>128</v>
+      </c>
+      <c r="C24" t="s" s="18">
+        <v>129</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="45" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="17" t="s">
+    <row r="25" ht="45" customHeight="1">
+      <c r="A25" t="s" s="4">
         <v>130</v>
+      </c>
+      <c r="B25" t="s" s="4">
+        <v>131</v>
+      </c>
+      <c r="C25" t="s" s="18">
+        <v>132</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1">
-      <c r="A26" s="4" t="s">
+    <row r="26" ht="30" customHeight="1">
+      <c r="A26" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>131</v>
+      <c r="C26" t="s" s="18">
+        <v>133</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="75" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="17" t="s">
+    <row r="27" ht="75" customHeight="1">
+      <c r="A27" t="s" s="4">
         <v>134</v>
+      </c>
+      <c r="B27" t="s" s="4">
+        <v>135</v>
+      </c>
+      <c r="C27" t="s" s="18">
+        <v>136</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1">
-      <c r="A28" s="4" t="s">
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s" s="4">
         <v>64</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>135</v>
+      <c r="C28" t="s" s="18">
+        <v>137</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1">
-      <c r="A29" s="4" t="s">
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>136</v>
+      <c r="C29" t="s" s="18">
+        <v>138</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="17" t="s">
+    <row r="30" ht="15" customHeight="1">
+      <c r="A30" t="s" s="4">
         <v>139</v>
+      </c>
+      <c r="B30" t="s" s="4">
+        <v>140</v>
+      </c>
+      <c r="C30" t="s" s="18">
+        <v>141</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1">
-      <c r="A31" s="4" t="s">
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" t="s" s="4">
         <v>67</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s" s="4">
         <v>68</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>140</v>
+      <c r="C31" t="s" s="18">
+        <v>142</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="17" t="s">
+    <row r="32" ht="30" customHeight="1">
+      <c r="A32" t="s" s="4">
         <v>143</v>
+      </c>
+      <c r="B32" t="s" s="4">
+        <v>144</v>
+      </c>
+      <c r="C32" t="s" s="18">
+        <v>145</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="17" t="s">
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" t="s" s="4">
         <v>146</v>
+      </c>
+      <c r="B33" t="s" s="4">
+        <v>147</v>
+      </c>
+      <c r="C33" t="s" s="18">
+        <v>148</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1">
-      <c r="A34" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34" s="17" t="s">
+    <row r="34" ht="30" customHeight="1">
+      <c r="A34" t="s" s="4">
         <v>149</v>
+      </c>
+      <c r="B34" t="s" s="4">
+        <v>150</v>
+      </c>
+      <c r="C34" t="s" s="18">
+        <v>151</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="30" customHeight="1">
-      <c r="A35" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C35" s="17" t="s">
+    <row r="35" ht="30" customHeight="1">
+      <c r="A35" t="s" s="4">
         <v>152</v>
+      </c>
+      <c r="B35" t="s" s="4">
+        <v>153</v>
+      </c>
+      <c r="C35" t="s" s="18">
+        <v>154</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" ht="30" customHeight="1">
-      <c r="A36" s="4" t="s">
+    <row r="36" ht="30" customHeight="1">
+      <c r="A36" t="s" s="4">
         <v>69</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s" s="4">
         <v>70</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>153</v>
+      <c r="C36" t="s" s="18">
+        <v>155</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1">
-      <c r="A37" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" s="17" t="s">
+    <row r="37" ht="30" customHeight="1">
+      <c r="A37" t="s" s="4">
         <v>156</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>157</v>
+      </c>
+      <c r="C37" t="s" s="18">
+        <v>158</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="30" customHeight="1">
-      <c r="A38" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="17" t="s">
+    <row r="38" ht="30" customHeight="1">
+      <c r="A38" t="s" s="4">
         <v>159</v>
+      </c>
+      <c r="B38" t="s" s="4">
+        <v>160</v>
+      </c>
+      <c r="C38" t="s" s="18">
+        <v>161</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" ht="30" customHeight="1">
-      <c r="A39" s="4" t="s">
+    <row r="39" ht="30" customHeight="1">
+      <c r="A39" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>160</v>
+      <c r="C39" t="s" s="18">
+        <v>162</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" ht="30" customHeight="1">
-      <c r="A40" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" s="17" t="s">
+    <row r="40" ht="30" customHeight="1">
+      <c r="A40" t="s" s="4">
         <v>163</v>
+      </c>
+      <c r="B40" t="s" s="4">
+        <v>164</v>
+      </c>
+      <c r="C40" t="s" s="18">
+        <v>165</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="30" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C41" s="17" t="s">
+    <row r="41" ht="30" customHeight="1">
+      <c r="A41" t="s" s="4">
         <v>166</v>
+      </c>
+      <c r="B41" t="s" s="4">
+        <v>167</v>
+      </c>
+      <c r="C41" t="s" s="18">
+        <v>168</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="30" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C42" s="17" t="s">
+    <row r="42" ht="30" customHeight="1">
+      <c r="A42" t="s" s="4">
         <v>169</v>
+      </c>
+      <c r="B42" t="s" s="4">
+        <v>170</v>
+      </c>
+      <c r="C42" t="s" s="18">
+        <v>171</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="30" customHeight="1">
-      <c r="A43" s="4" t="s">
+    <row r="43" ht="30" customHeight="1">
+      <c r="A43" t="s" s="4">
         <v>73</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>170</v>
+      <c r="C43" t="s" s="18">
+        <v>172</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
US09 & US08 changes updated
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezhil\Documents\agile\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" r:id="rId4"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId5"/>
-    <sheet name="Burndown" sheetId="3" r:id="rId6"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId7"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId8"/>
-    <sheet name="Sprint3" sheetId="6" r:id="rId9"/>
-    <sheet name="Sprint4" sheetId="7" r:id="rId10"/>
-    <sheet name="Stories" sheetId="8" r:id="rId11"/>
+    <sheet name="Team" sheetId="1" r:id="rId1"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
+    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
+    <sheet name="Stories" sheetId="8" r:id="rId8"/>
   </sheets>
+  <calcPr calcId="171027" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="173">
   <si>
     <t>Initials</t>
   </si>
@@ -86,7 +94,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="11"/>
         <rFont val="Verdana"/>
@@ -253,7 +261,6 @@
   <si>
     <t>Reject illegitimate dates</t>
   </si>
-  <si/>
   <si>
     <t>Date</t>
   </si>
@@ -300,308 +307,303 @@
     <t>Avoid:</t>
   </si>
   <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Story Description</t>
+  </si>
+  <si>
+    <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
+  </si>
+  <si>
+    <t>Birth should occur before marriage of an individual</t>
+  </si>
+  <si>
+    <t>Birth should occur before death of an individual</t>
+  </si>
+  <si>
+    <t>Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
+  </si>
+  <si>
+    <t>Marriage should occur before death of either spouse</t>
+  </si>
+  <si>
+    <t>Divorce can only occur before death of both spouses</t>
+  </si>
+  <si>
+    <t>Death should be less than 150 years after birth for dead people, and current date should be less than 150 years after birth for all living people</t>
+  </si>
+  <si>
+    <t>Child should be born after marriage of parents (and before their divorce)</t>
+  </si>
+  <si>
+    <t>Child should be born before death of mother and before 9 months after death of father</t>
+  </si>
+  <si>
+    <t>Marriage should be at least 14 years after birth of both spouses</t>
+  </si>
+  <si>
+    <t>US11</t>
+  </si>
+  <si>
+    <t>No bigamy</t>
+  </si>
+  <si>
+    <t>Marriage should not occur during marriage to another spouse</t>
+  </si>
+  <si>
+    <t>US12</t>
+  </si>
+  <si>
+    <t>Parents not too old</t>
+  </si>
+  <si>
+    <t>Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
+  </si>
+  <si>
+    <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart</t>
+  </si>
+  <si>
+    <t>No more than five siblings should be born at the same time</t>
+  </si>
+  <si>
+    <t>US15</t>
+  </si>
+  <si>
+    <t>Fewer than 15 siblings</t>
+  </si>
+  <si>
+    <t>There should be fewer than 15 siblings in a family</t>
+  </si>
+  <si>
+    <t>US16</t>
+  </si>
+  <si>
+    <t>Male last names</t>
+  </si>
+  <si>
+    <t>All male members of a family should have the same last name</t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>No marriages to descendants</t>
+  </si>
+  <si>
+    <t>Parents should not marry any of their descendants</t>
+  </si>
+  <si>
+    <t>Siblings should not marry one another</t>
+  </si>
+  <si>
+    <t>First cousins should not marry one another</t>
+  </si>
+  <si>
+    <t>Aunts and uncles should not marry their nieces or nephews</t>
+  </si>
+  <si>
+    <t>Husband in family should be male and wife in family should be female</t>
+  </si>
+  <si>
+    <t>All individual IDs should be unique and all family IDs should be unique</t>
+  </si>
+  <si>
+    <t>US23</t>
+  </si>
+  <si>
+    <t>Unique name and birth date</t>
+  </si>
+  <si>
+    <t>No more than one individual with the same name and birth date should appear in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>US24</t>
+  </si>
+  <si>
+    <t>Unique families by spouses</t>
+  </si>
+  <si>
+    <t>No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>No more than one child with the same name and birth date should appear in a family</t>
+  </si>
+  <si>
+    <t>US26</t>
+  </si>
+  <si>
+    <t>Corresponding entries</t>
+  </si>
+  <si>
+    <t>All family roles (spouse, child) specified in an individual record should have corresponding entries in those family records, and all individual roles (spouse, child) specified in family records should have corresponding entries in those individual's records</t>
+  </si>
+  <si>
+    <t>Include person's current age when listing individuals</t>
+  </si>
+  <si>
+    <t>List siblings in families by age</t>
+  </si>
+  <si>
+    <t>US29</t>
+  </si>
+  <si>
+    <t>List deceased</t>
+  </si>
+  <si>
+    <t>List all deceased individuals in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all living married people in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>US31</t>
+  </si>
+  <si>
+    <t>List living single</t>
+  </si>
+  <si>
+    <t>List all living people over 30 who have never been married in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>US32</t>
+  </si>
+  <si>
+    <t>List multiple births</t>
+  </si>
+  <si>
+    <t>List all multiple births in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>US33</t>
+  </si>
+  <si>
+    <t>List orphans</t>
+  </si>
+  <si>
+    <t>List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>US34</t>
+  </si>
+  <si>
+    <t>List large age differences</t>
+  </si>
+  <si>
+    <t>List all couples who were married when the older spouse was more than twice as old as the younger spouse</t>
+  </si>
+  <si>
+    <t>List all people in a GEDCOM file who were born in the last 30 days</t>
+  </si>
+  <si>
+    <t>US36</t>
+  </si>
+  <si>
+    <t>List recent deaths</t>
+  </si>
+  <si>
+    <t>List all people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t>US37</t>
+  </si>
+  <si>
+    <t>List recent survivors</t>
+  </si>
+  <si>
+    <t>List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t>List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
+  </si>
+  <si>
+    <t>US39</t>
+  </si>
+  <si>
+    <t>List upcoming anniversaries</t>
+  </si>
+  <si>
+    <t>List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
+  </si>
+  <si>
+    <t>US40</t>
+  </si>
+  <si>
+    <t>Include input line numbers</t>
+  </si>
+  <si>
+    <t>List line numbers from GEDCOM source file when reporting errors</t>
+  </si>
+  <si>
+    <t>US41</t>
+  </si>
+  <si>
+    <t>Include partial dates</t>
+  </si>
+  <si>
+    <t>Accept and use dates without days or without days and months</t>
+  </si>
+  <si>
+    <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
     <t>done</t>
   </si>
   <si>
-    <t>pending</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Story Description</t>
-  </si>
-  <si>
-    <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
-  </si>
-  <si>
-    <t>Birth should occur before marriage of an individual</t>
-  </si>
-  <si>
-    <t>Birth should occur before death of an individual</t>
-  </si>
-  <si>
-    <t>Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
-  </si>
-  <si>
-    <t>Marriage should occur before death of either spouse</t>
-  </si>
-  <si>
-    <t>Divorce can only occur before death of both spouses</t>
-  </si>
-  <si>
-    <t>Death should be less than 150 years after birth for dead people, and current date should be less than 150 years after birth for all living people</t>
-  </si>
-  <si>
-    <t>Child should be born after marriage of parents (and before their divorce)</t>
-  </si>
-  <si>
-    <t>Child should be born before death of mother and before 9 months after death of father</t>
-  </si>
-  <si>
-    <t>Marriage should be at least 14 years after birth of both spouses</t>
-  </si>
-  <si>
-    <t>US11</t>
-  </si>
-  <si>
-    <t>No bigamy</t>
-  </si>
-  <si>
-    <t>Marriage should not occur during marriage to another spouse</t>
-  </si>
-  <si>
-    <t>US12</t>
-  </si>
-  <si>
-    <t>Parents not too old</t>
-  </si>
-  <si>
-    <t>Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
-  </si>
-  <si>
-    <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart</t>
-  </si>
-  <si>
-    <t>No more than five siblings should be born at the same time</t>
-  </si>
-  <si>
-    <t>US15</t>
-  </si>
-  <si>
-    <t>Fewer than 15 siblings</t>
-  </si>
-  <si>
-    <t>There should be fewer than 15 siblings in a family</t>
-  </si>
-  <si>
-    <t>US16</t>
-  </si>
-  <si>
-    <t>Male last names</t>
-  </si>
-  <si>
-    <t>All male members of a family should have the same last name</t>
-  </si>
-  <si>
-    <t>US17</t>
-  </si>
-  <si>
-    <t>No marriages to descendants</t>
-  </si>
-  <si>
-    <t>Parents should not marry any of their descendants</t>
-  </si>
-  <si>
-    <t>Siblings should not marry one another</t>
-  </si>
-  <si>
-    <t>First cousins should not marry one another</t>
-  </si>
-  <si>
-    <t>Aunts and uncles should not marry their nieces or nephews</t>
-  </si>
-  <si>
-    <t>Husband in family should be male and wife in family should be female</t>
-  </si>
-  <si>
-    <t>All individual IDs should be unique and all family IDs should be unique</t>
-  </si>
-  <si>
-    <t>US23</t>
-  </si>
-  <si>
-    <t>Unique name and birth date</t>
-  </si>
-  <si>
-    <t>No more than one individual with the same name and birth date should appear in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>US24</t>
-  </si>
-  <si>
-    <t>Unique families by spouses</t>
-  </si>
-  <si>
-    <t>No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>No more than one child with the same name and birth date should appear in a family</t>
-  </si>
-  <si>
-    <t>US26</t>
-  </si>
-  <si>
-    <t>Corresponding entries</t>
-  </si>
-  <si>
-    <t>All family roles (spouse, child) specified in an individual record should have corresponding entries in those family records, and all individual roles (spouse, child) specified in family records should have corresponding entries in those individual's records</t>
-  </si>
-  <si>
-    <t>Include person's current age when listing individuals</t>
-  </si>
-  <si>
-    <t>List siblings in families by age</t>
-  </si>
-  <si>
-    <t>US29</t>
-  </si>
-  <si>
-    <t>List deceased</t>
-  </si>
-  <si>
-    <t>List all deceased individuals in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all living married people in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>US31</t>
-  </si>
-  <si>
-    <t>List living single</t>
-  </si>
-  <si>
-    <t>List all living people over 30 who have never been married in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>US32</t>
-  </si>
-  <si>
-    <t>List multiple births</t>
-  </si>
-  <si>
-    <t>List all multiple births in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>US33</t>
-  </si>
-  <si>
-    <t>List orphans</t>
-  </si>
-  <si>
-    <t>List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>US34</t>
-  </si>
-  <si>
-    <t>List large age differences</t>
-  </si>
-  <si>
-    <t>List all couples who were married when the older spouse was more than twice as old as the younger spouse</t>
-  </si>
-  <si>
-    <t>List all people in a GEDCOM file who were born in the last 30 days</t>
-  </si>
-  <si>
-    <t>US36</t>
-  </si>
-  <si>
-    <t>List recent deaths</t>
-  </si>
-  <si>
-    <t>List all people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t>US37</t>
-  </si>
-  <si>
-    <t>List recent survivors</t>
-  </si>
-  <si>
-    <t>List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t>List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
-  </si>
-  <si>
-    <t>US39</t>
-  </si>
-  <si>
-    <t>List upcoming anniversaries</t>
-  </si>
-  <si>
-    <t>List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
-  </si>
-  <si>
-    <t>US40</t>
-  </si>
-  <si>
-    <t>Include input line numbers</t>
-  </si>
-  <si>
-    <t>List line numbers from GEDCOM source file when reporting errors</t>
-  </si>
-  <si>
-    <t>US41</t>
-  </si>
-  <si>
-    <t>Include partial dates</t>
-  </si>
-  <si>
-    <t>Accept and use dates without days or without days and months</t>
-  </si>
-  <si>
-    <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="m/d"/>
-    <numFmt numFmtId="60" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Cambria"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Cambria"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -642,100 +644,154 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+  <cellStyleXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ff888888"/>
-      <rgbColor rgb="ff4a7ebb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF888888"/>
+      <rgbColor rgb="FF4A7EBB"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="18"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -744,10 +800,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0836907"/>
-          <c:y val="0.0608311"/>
-          <c:w val="0.911309"/>
-          <c:h val="0.828202"/>
+          <c:x val="8.3645800000000006E-2"/>
+          <c:y val="6.0070699999999998E-2"/>
+          <c:w val="0.911354"/>
+          <c:h val="0.83019299999999996"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -760,9 +816,6 @@
             <c:v>Series1</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
             <a:ln w="28575" cap="flat">
               <a:solidFill>
                 <a:srgbClr val="4A7EBB"/>
@@ -774,7 +827,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="4"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -789,88 +842,70 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Helvetica"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>'Burndown'!$A$2:$A$7</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Burndown!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2/9</c:v>
+                  <c:v>40947</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/23</c:v>
+                  <c:v>40961</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>15-Mar</c:v>
+                <c:pt idx="2" formatCode="d\-mmm">
+                  <c:v>40982</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown'!$B$2:$B$7</c:f>
+              <c:f>Burndown!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:ptCount val="3"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.000000</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.000000</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.000000</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-32A8-4804-BF13-24DEC399267B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="2094734552"/>
-        <c:axId val="2094734553"/>
+        <c:smooth val="0"/>
+        <c:axId val="2107830952"/>
+        <c:axId val="2107827928"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="2094734552"/>
+      <c:dateAx>
+        <c:axId val="2107830952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -888,23 +923,24 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734553"/>
+        <c:crossAx val="2107827928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="2094734553"/>
+        <c:axId val="2107827928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,16 +975,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734552"/>
+        <c:crossAx val="2107830952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="6"/>
@@ -967,6 +1004,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -981,36 +1019,41 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>510977</xdr:colOff>
+      <xdr:colOff>510978</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>107516</xdr:colOff>
+      <xdr:colOff>109574</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>68222</xdr:rowOff>
+      <xdr:rowOff>97293</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1323777" y="1715049"/>
-        <a:ext cx="3838340" cy="2296524"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1020,7 +1063,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1146,7 +1189,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1155,7 +1198,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1164,7 +1207,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1238,7 +1281,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1246,7 +1289,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1265,7 +1308,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1295,7 +1338,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1321,7 +1364,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1347,7 +1390,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1373,7 +1416,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1399,7 +1442,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1425,7 +1468,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1451,7 +1494,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1477,7 +1520,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1503,7 +1546,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1516,9 +1559,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1533,7 +1582,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1541,7 +1590,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1560,7 +1609,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1586,7 +1635,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1612,7 +1661,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1638,7 +1687,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1664,7 +1713,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1690,7 +1739,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1716,7 +1765,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1742,7 +1791,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1768,7 +1817,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1794,7 +1843,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1807,9 +1856,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1823,7 +1878,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1842,7 +1897,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1872,7 +1927,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1898,7 +1953,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1924,7 +1979,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1950,7 +2005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1976,7 +2031,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2002,7 +2057,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2028,7 +2083,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2054,7 +2109,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2080,7 +2135,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2093,140 +2148,147 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.35156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.3046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3046875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.15234375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3828125" style="1" customWidth="1"/>
     <col min="6" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s" s="4">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="4">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s" s="4">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s" s="4">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s" s="4">
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2235,7 +2297,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2243,369 +2305,371 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.35156" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.67188" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="5" customWidth="1"/>
-    <col min="4" max="4" width="6.67188" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.67188" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.3046875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.69140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.3828125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.69140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.69140625" style="5" customWidth="1"/>
     <col min="6" max="256" width="11" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s" s="4">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" t="s" s="4">
+      <c r="B9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s" s="4">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="C10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" t="s" s="4">
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>3</v>
       </c>
-      <c r="B11" t="s" s="4">
+      <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s" s="4">
+      <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s" s="4">
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B12" t="s" s="4">
+      <c r="B12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s" s="4">
+      <c r="C12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s" s="4">
+      <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>3</v>
       </c>
-      <c r="B13" t="s" s="4">
+      <c r="B13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s" s="4">
+      <c r="C13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s" s="4">
+      <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2</v>
       </c>
-      <c r="B14" t="s" s="4">
+      <c r="B14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s" s="4">
+      <c r="C14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s" s="4">
+      <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2</v>
       </c>
-      <c r="B15" t="s" s="4">
+      <c r="B15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s" s="4">
+      <c r="C15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D15" t="s" s="4">
+      <c r="D15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" t="s" s="4">
+      <c r="B16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s" s="4">
+      <c r="C16" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" t="s" s="4">
+      <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s" s="4">
+      <c r="C17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D17" t="s" s="4">
+      <c r="D17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="B18" t="s" s="4">
+      <c r="B18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s" s="4">
+      <c r="C18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D18" t="s" s="4">
+      <c r="D18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>2</v>
       </c>
-      <c r="B19" t="s" s="4">
+      <c r="B19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C19" t="s" s="4">
+      <c r="C19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D19" t="s" s="4">
+      <c r="D19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>2</v>
       </c>
-      <c r="B20" t="s" s="4">
+      <c r="B20" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s" s="4">
+      <c r="C20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D20" t="s" s="4">
+      <c r="D20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>2</v>
       </c>
-      <c r="B21" t="s" s="4">
+      <c r="B21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s" s="4">
+      <c r="C21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D21" t="s" s="4">
+      <c r="D21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>3</v>
       </c>
-      <c r="B22" t="s" s="4">
+      <c r="B22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s" s="4">
+      <c r="C22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D22" t="s" s="4">
+      <c r="D22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
-      <c r="B23" t="s" s="4">
+      <c r="B23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s" s="4">
+      <c r="C23" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>3</v>
       </c>
-      <c r="B24" t="s" s="4">
+      <c r="B24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s" s="4">
+      <c r="C24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s" s="4">
+      <c r="D24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" t="s" s="4">
+      <c r="B25" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s" s="4">
+      <c r="C25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="3"/>
@@ -2613,7 +2677,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2621,45 +2685,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6719" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.6719" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="7.17188" style="6" customWidth="1"/>
-    <col min="5" max="5" width="6.85156" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11" style="6" customWidth="1"/>
-    <col min="8" max="256" width="11" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.69140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.3828125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.3828125" style="6" customWidth="1"/>
+    <col min="7" max="256" width="11" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s" s="2">
-        <v>81</v>
-      </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" ht="13.5" customHeight="1">
+    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>40947</v>
       </c>
@@ -2674,7 +2739,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" ht="13.5" customHeight="1">
+    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>40961</v>
       </c>
@@ -2693,12 +2758,12 @@
       </c>
       <c r="F3" s="8">
         <f>(D3-D2)/E3*60</f>
-        <v>125</v>
+        <v>125.00000000000001</v>
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="9">
+    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
         <v>40982</v>
       </c>
       <c r="B4" s="3">
@@ -2715,11 +2780,11 @@
       </c>
       <c r="F4" s="8">
         <f>(D4-D3)/E4*60</f>
-        <v>76.59999999999999</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" ht="13.5" customHeight="1">
+    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2728,7 +2793,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" ht="13.5" customHeight="1">
+    <row r="6" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2737,7 +2802,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" ht="13.5" customHeight="1">
+    <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2746,7 +2811,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" ht="13.5" customHeight="1">
+    <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2755,7 +2820,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" ht="13.5" customHeight="1">
+    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2764,7 +2829,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" ht="13.5" customHeight="1">
+    <row r="10" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2773,7 +2838,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" ht="13.5" customHeight="1">
+    <row r="11" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2782,7 +2847,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" ht="13.5" customHeight="1">
+    <row r="12" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2791,7 +2856,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" ht="13.5" customHeight="1">
+    <row r="13" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2800,7 +2865,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" ht="13.5" customHeight="1">
+    <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2809,7 +2874,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" ht="13.5" customHeight="1">
+    <row r="15" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2818,7 +2883,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" ht="13.5" customHeight="1">
+    <row r="16" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2827,7 +2892,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" ht="13.5" customHeight="1">
+    <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2836,7 +2901,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" ht="13.5" customHeight="1">
+    <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2845,7 +2910,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" ht="13.5" customHeight="1">
+    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2854,7 +2919,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" ht="13.5" customHeight="1">
+    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2863,7 +2928,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" ht="13.5" customHeight="1">
+    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2872,7 +2937,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" ht="13.5" customHeight="1">
+    <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2881,7 +2946,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" ht="13.5" customHeight="1">
+    <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2890,7 +2955,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" ht="13.5" customHeight="1">
+    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2899,7 +2964,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" ht="13.5" customHeight="1">
+    <row r="25" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2908,7 +2973,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" ht="13.5" customHeight="1">
+    <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2919,7 +2984,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2928,62 +2993,63 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.67188" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="6.67188" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.3516" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.3516" style="10" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="10" customWidth="1"/>
-    <col min="8" max="8" width="9.35156" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.6719" style="10" customWidth="1"/>
-    <col min="10" max="256" width="11" style="10" customWidth="1"/>
+    <col min="1" max="1" width="7.69140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="24.3828125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.69140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11" style="9" customWidth="1"/>
+    <col min="5" max="6" width="10.3046875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="8.3828125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="9.3046875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.69140625" style="9" customWidth="1"/>
+    <col min="10" max="256" width="11" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="11">
+      <c r="B1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s" s="12">
+      <c r="E1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s" s="12">
+      <c r="G1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s" s="12">
+      <c r="H1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s" s="12">
+      <c r="I1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s" s="12">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3"/>
@@ -2999,18 +3065,18 @@
       <c r="H2" s="3">
         <v>30</v>
       </c>
-      <c r="I2" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="I2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="3"/>
@@ -3026,18 +3092,18 @@
       <c r="H3" s="3">
         <v>10</v>
       </c>
-      <c r="I3" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="I3" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="3"/>
@@ -3053,18 +3119,18 @@
       <c r="H4" s="3">
         <v>60</v>
       </c>
-      <c r="I4" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="I4" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="3"/>
@@ -3080,18 +3146,18 @@
       <c r="H5" s="3">
         <v>40</v>
       </c>
-      <c r="I5" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
+      <c r="I5" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="3"/>
@@ -3107,18 +3173,18 @@
       <c r="H6" s="3">
         <v>60</v>
       </c>
-      <c r="I6" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
+      <c r="I6" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3"/>
@@ -3134,13 +3200,13 @@
       <c r="H7" s="3">
         <v>5</v>
       </c>
-      <c r="I7" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
+      <c r="I7" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -3149,9 +3215,9 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -3160,9 +3226,9 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -3171,9 +3237,9 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3182,9 +3248,9 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -3193,10 +3259,10 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" t="s" s="11">
-        <v>88</v>
+      <c r="B13" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3206,9 +3272,9 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="11"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -3217,10 +3283,10 @@
       <c r="H14" s="3"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" t="s" s="11">
-        <v>89</v>
+      <c r="B15" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -3230,9 +3296,9 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="13"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -3241,9 +3307,9 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="13"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -3252,9 +3318,9 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="13"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3263,10 +3329,10 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" t="s" s="11">
-        <v>90</v>
+      <c r="B19" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -3278,7 +3344,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3286,66 +3352,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="14" customWidth="1"/>
-    <col min="2" max="2" width="24.6719" style="14" customWidth="1"/>
-    <col min="3" max="3" width="11" style="14" customWidth="1"/>
-    <col min="4" max="4" width="11" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11" style="14" customWidth="1"/>
-    <col min="6" max="6" width="11" style="14" customWidth="1"/>
-    <col min="7" max="7" width="11" style="14" customWidth="1"/>
-    <col min="8" max="8" width="11" style="14" customWidth="1"/>
-    <col min="9" max="9" width="11" style="14" customWidth="1"/>
-    <col min="10" max="256" width="11" style="14" customWidth="1"/>
+    <col min="1" max="1" width="11" style="13" customWidth="1"/>
+    <col min="2" max="2" width="24.69140625" style="13" customWidth="1"/>
+    <col min="3" max="256" width="11" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="11">
+      <c r="B1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s" s="12">
+      <c r="E1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s" s="12">
+      <c r="G1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s" s="12">
+      <c r="H1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s" s="12">
+      <c r="I1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s" s="12">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="4">
-        <v>91</v>
+      <c r="D2" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="E2" s="3">
         <v>12</v>
@@ -3359,22 +3420,22 @@
       <c r="H2" s="3">
         <v>70</v>
       </c>
-      <c r="I2" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="I2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s" s="4">
-        <v>92</v>
+      <c r="D3" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="E3" s="3">
         <v>15</v>
@@ -3388,20 +3449,22 @@
       <c r="H3" s="3">
         <v>120</v>
       </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="I3" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="4">
-        <v>93</v>
+      <c r="D4" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="E4" s="3">
         <v>5</v>
@@ -3415,22 +3478,22 @@
       <c r="H4" s="3">
         <v>48</v>
       </c>
-      <c r="I4" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="I4" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s" s="4">
-        <v>93</v>
+      <c r="D5" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="E5" s="3">
         <v>20</v>
@@ -3444,22 +3507,22 @@
       <c r="H5" s="3">
         <v>30</v>
       </c>
-      <c r="I5" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
+      <c r="I5" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s" s="4">
-        <v>93</v>
+      <c r="D6" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="E6" s="3">
         <v>20</v>
@@ -3473,22 +3536,22 @@
       <c r="H6" s="3">
         <v>45</v>
       </c>
-      <c r="I6" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
+      <c r="I6" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s" s="4">
-        <v>93</v>
+      <c r="D7" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="E7" s="3">
         <v>7</v>
@@ -3502,11 +3565,11 @@
       <c r="H7" s="3">
         <v>25</v>
       </c>
-      <c r="I7" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
+      <c r="I7" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3517,7 +3580,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3528,7 +3591,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3541,7 +3604,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3549,96 +3612,115 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="15" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="15" customWidth="1"/>
-    <col min="3" max="3" width="11" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11" style="15" customWidth="1"/>
-    <col min="5" max="5" width="11" style="15" customWidth="1"/>
-    <col min="6" max="6" width="11" style="15" customWidth="1"/>
-    <col min="7" max="7" width="11" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11" style="15" customWidth="1"/>
-    <col min="9" max="9" width="11" style="15" customWidth="1"/>
-    <col min="10" max="256" width="11" style="15" customWidth="1"/>
+    <col min="1" max="1" width="11" style="14" customWidth="1"/>
+    <col min="2" max="2" width="26.3828125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="256" width="11" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="11">
+      <c r="B1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s" s="12">
+      <c r="E1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s" s="12">
+      <c r="G1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s" s="12">
+      <c r="H1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s" s="12">
+      <c r="I1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s" s="12">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="3">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45</v>
+      </c>
+      <c r="G2" s="3">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3">
+        <v>45</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s" s="4">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s" s="4">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s" s="4">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="D3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3">
         <v>45</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>30</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="3"/>
@@ -3648,14 +3730,14 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="4">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3"/>
@@ -3665,65 +3747,41 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s" s="4">
-        <v>91</v>
-      </c>
-      <c r="E6" s="3">
-        <v>20</v>
-      </c>
-      <c r="F6" s="3">
-        <v>30</v>
-      </c>
-      <c r="G6" s="3">
-        <v>30</v>
-      </c>
-      <c r="H6" s="3">
-        <v>30</v>
-      </c>
-      <c r="I6" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s" s="4">
-        <v>91</v>
-      </c>
-      <c r="E7" s="3">
-        <v>21</v>
-      </c>
-      <c r="F7" s="3">
-        <v>30</v>
-      </c>
-      <c r="G7" s="3">
-        <v>28</v>
-      </c>
-      <c r="H7" s="3">
-        <v>30</v>
-      </c>
-      <c r="I7" t="s" s="4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3734,7 +3792,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3745,7 +3803,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3758,7 +3816,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3766,55 +3824,46 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="16" customWidth="1"/>
-    <col min="2" max="2" width="11" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11" style="16" customWidth="1"/>
-    <col min="4" max="4" width="11" style="16" customWidth="1"/>
-    <col min="5" max="5" width="11" style="16" customWidth="1"/>
-    <col min="6" max="6" width="11" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11" style="16" customWidth="1"/>
-    <col min="8" max="8" width="11" style="16" customWidth="1"/>
-    <col min="9" max="9" width="11" style="16" customWidth="1"/>
-    <col min="10" max="256" width="11" style="16" customWidth="1"/>
+    <col min="1" max="256" width="11" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="11">
+      <c r="B1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s" s="12">
+      <c r="E1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s" s="12">
+      <c r="G1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s" s="12">
+      <c r="H1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s" s="12">
+      <c r="I1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s" s="12">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3825,7 +3874,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3836,7 +3885,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3847,7 +3896,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3858,7 +3907,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3869,7 +3918,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3880,7 +3929,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3891,7 +3940,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3902,7 +3951,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3915,7 +3964,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3923,583 +3972,581 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV43"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="17" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="49.3516" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11" style="17" customWidth="1"/>
-    <col min="5" max="5" width="11" style="17" customWidth="1"/>
-    <col min="6" max="256" width="11" style="17" customWidth="1"/>
+    <col min="1" max="1" width="11" style="16" customWidth="1"/>
+    <col min="2" max="2" width="24.3828125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="49.3046875" style="16" customWidth="1"/>
+    <col min="4" max="256" width="11" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s" s="11">
-        <v>94</v>
+      <c r="C1" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" ht="30" customHeight="1">
-      <c r="A2" t="s" s="4">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s" s="18">
-        <v>95</v>
+      <c r="C2" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s" s="18">
-        <v>96</v>
+      <c r="C3" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s" s="18">
-        <v>97</v>
+      <c r="C4" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" ht="30" customHeight="1">
-      <c r="A5" t="s" s="4">
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s" s="18">
-        <v>98</v>
+      <c r="C5" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s" s="18">
-        <v>99</v>
+      <c r="C6" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s" s="18">
-        <v>100</v>
+      <c r="C7" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" ht="45" customHeight="1">
-      <c r="A8" t="s" s="4">
+    <row r="8" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s" s="18">
-        <v>101</v>
+      <c r="C8" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" ht="30" customHeight="1">
-      <c r="A9" t="s" s="4">
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s" s="4">
+      <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s" s="18">
-        <v>102</v>
+      <c r="C9" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="30" customHeight="1">
-      <c r="A10" t="s" s="4">
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C10" t="s" s="18">
-        <v>103</v>
+      <c r="C10" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" ht="30" customHeight="1">
-      <c r="A11" t="s" s="4">
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s" s="4">
+      <c r="B11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s" s="18">
-        <v>104</v>
+      <c r="C11" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" ht="30" customHeight="1">
-      <c r="A12" t="s" s="4">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>105</v>
-      </c>
-      <c r="B12" t="s" s="4">
-        <v>106</v>
-      </c>
-      <c r="C12" t="s" s="18">
-        <v>107</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" ht="45" customHeight="1">
-      <c r="A13" t="s" s="4">
+    <row r="13" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="B13" t="s" s="4">
-        <v>109</v>
-      </c>
-      <c r="C13" t="s" s="18">
-        <v>110</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" ht="30" customHeight="1">
-      <c r="A14" t="s" s="4">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s" s="4">
+      <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s" s="18">
-        <v>111</v>
+      <c r="C14" s="17" t="s">
+        <v>109</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="4">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s" s="4">
+      <c r="B15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15" t="s" s="18">
-        <v>112</v>
+      <c r="C15" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="4">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>113</v>
-      </c>
-      <c r="B16" t="s" s="4">
-        <v>114</v>
-      </c>
-      <c r="C16" t="s" s="18">
-        <v>115</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" ht="30" customHeight="1">
-      <c r="A17" t="s" s="4">
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="B17" t="s" s="4">
-        <v>117</v>
-      </c>
-      <c r="C17" t="s" s="18">
-        <v>118</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="4">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>119</v>
-      </c>
-      <c r="B18" t="s" s="4">
-        <v>120</v>
-      </c>
-      <c r="C18" t="s" s="18">
-        <v>121</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="4">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s" s="4">
+      <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s" s="18">
-        <v>122</v>
+      <c r="C19" s="17" t="s">
+        <v>120</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="4">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s" s="4">
+      <c r="B20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C20" t="s" s="18">
-        <v>123</v>
+      <c r="C20" s="17" t="s">
+        <v>121</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
-      <c r="A21" t="s" s="4">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s" s="4">
+      <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C21" t="s" s="18">
-        <v>124</v>
+      <c r="C21" s="17" t="s">
+        <v>122</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" ht="30" customHeight="1">
-      <c r="A22" t="s" s="4">
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B22" t="s" s="4">
+      <c r="B22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C22" t="s" s="18">
-        <v>125</v>
+      <c r="C22" s="17" t="s">
+        <v>123</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" ht="30" customHeight="1">
-      <c r="A23" t="s" s="4">
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B23" t="s" s="4">
+      <c r="B23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C23" t="s" s="18">
-        <v>126</v>
+      <c r="C23" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" ht="30" customHeight="1">
-      <c r="A24" t="s" s="4">
+    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>127</v>
-      </c>
-      <c r="B24" t="s" s="4">
-        <v>128</v>
-      </c>
-      <c r="C24" t="s" s="18">
-        <v>129</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" ht="45" customHeight="1">
-      <c r="A25" t="s" s="4">
+    <row r="25" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>130</v>
-      </c>
-      <c r="B25" t="s" s="4">
-        <v>131</v>
-      </c>
-      <c r="C25" t="s" s="18">
-        <v>132</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" ht="30" customHeight="1">
-      <c r="A26" t="s" s="4">
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s" s="4">
+      <c r="B26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C26" t="s" s="18">
-        <v>133</v>
+      <c r="C26" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" ht="75" customHeight="1">
-      <c r="A27" t="s" s="4">
+    <row r="27" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="B27" t="s" s="4">
-        <v>135</v>
-      </c>
-      <c r="C27" t="s" s="18">
-        <v>136</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" ht="15" customHeight="1">
-      <c r="A28" t="s" s="4">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B28" t="s" s="4">
+      <c r="B28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C28" t="s" s="18">
-        <v>137</v>
+      <c r="C28" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" ht="15" customHeight="1">
-      <c r="A29" t="s" s="4">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B29" t="s" s="4">
+      <c r="B29" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C29" t="s" s="18">
-        <v>138</v>
+      <c r="C29" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" ht="15" customHeight="1">
-      <c r="A30" t="s" s="4">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>139</v>
-      </c>
-      <c r="B30" t="s" s="4">
-        <v>140</v>
-      </c>
-      <c r="C30" t="s" s="18">
-        <v>141</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" ht="15" customHeight="1">
-      <c r="A31" t="s" s="4">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B31" t="s" s="4">
+      <c r="B31" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s" s="18">
-        <v>142</v>
+      <c r="C31" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" ht="30" customHeight="1">
-      <c r="A32" t="s" s="4">
+    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="B32" t="s" s="4">
-        <v>144</v>
-      </c>
-      <c r="C32" t="s" s="18">
-        <v>145</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" ht="15" customHeight="1">
-      <c r="A33" t="s" s="4">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="B33" t="s" s="4">
-        <v>147</v>
-      </c>
-      <c r="C33" t="s" s="18">
-        <v>148</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" ht="30" customHeight="1">
-      <c r="A34" t="s" s="4">
+    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="B34" t="s" s="4">
-        <v>150</v>
-      </c>
-      <c r="C34" t="s" s="18">
-        <v>151</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" ht="30" customHeight="1">
-      <c r="A35" t="s" s="4">
+    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="B35" t="s" s="4">
-        <v>153</v>
-      </c>
-      <c r="C35" t="s" s="18">
-        <v>154</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" ht="30" customHeight="1">
-      <c r="A36" t="s" s="4">
+    <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B36" t="s" s="4">
+      <c r="B36" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C36" t="s" s="18">
-        <v>155</v>
+      <c r="C36" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" ht="30" customHeight="1">
-      <c r="A37" t="s" s="4">
+    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="B37" t="s" s="4">
-        <v>157</v>
-      </c>
-      <c r="C37" t="s" s="18">
-        <v>158</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" ht="30" customHeight="1">
-      <c r="A38" t="s" s="4">
+    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>159</v>
-      </c>
-      <c r="B38" t="s" s="4">
-        <v>160</v>
-      </c>
-      <c r="C38" t="s" s="18">
-        <v>161</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" ht="30" customHeight="1">
-      <c r="A39" t="s" s="4">
+    <row r="39" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B39" t="s" s="4">
+      <c r="B39" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C39" t="s" s="18">
-        <v>162</v>
+      <c r="C39" s="17" t="s">
+        <v>160</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" ht="30" customHeight="1">
-      <c r="A40" t="s" s="4">
+    <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>163</v>
-      </c>
-      <c r="B40" t="s" s="4">
-        <v>164</v>
-      </c>
-      <c r="C40" t="s" s="18">
-        <v>165</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" ht="30" customHeight="1">
-      <c r="A41" t="s" s="4">
+    <row r="41" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="B41" t="s" s="4">
-        <v>167</v>
-      </c>
-      <c r="C41" t="s" s="18">
-        <v>168</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" ht="30" customHeight="1">
-      <c r="A42" t="s" s="4">
+    <row r="42" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>169</v>
-      </c>
-      <c r="B42" t="s" s="4">
-        <v>170</v>
-      </c>
-      <c r="C42" t="s" s="18">
-        <v>171</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" ht="30" customHeight="1">
-      <c r="A43" t="s" s="4">
+    <row r="43" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B43" t="s" s="4">
+      <c r="B43" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C43" t="s" s="18">
-        <v>172</v>
+      <c r="C43" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
added updated report and resutls
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,33 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr date1904="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezhil\Documents\agile\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" r:id="rId1"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
-    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
-    <sheet name="Stories" sheetId="8" r:id="rId8"/>
+    <sheet name="Team" sheetId="1" r:id="rId4"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId5"/>
+    <sheet name="Burndown" sheetId="3" r:id="rId6"/>
+    <sheet name="Sprint1" sheetId="4" r:id="rId7"/>
+    <sheet name="Sprint2" sheetId="5" r:id="rId8"/>
+    <sheet name="Sprint3" sheetId="6" r:id="rId9"/>
+    <sheet name="Sprint4" sheetId="7" r:id="rId10"/>
+    <sheet name="Stories" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="178">
   <si>
     <t>Initials</t>
   </si>
@@ -94,7 +86,7 @@
   <si>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color indexed="11"/>
         <rFont val="Verdana"/>
@@ -261,6 +253,7 @@
   <si>
     <t>Reject illegitimate dates</t>
   </si>
+  <si/>
   <si>
     <t>Date</t>
   </si>
@@ -307,12 +300,46 @@
     <t>Avoid:</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
     <t>pending</t>
   </si>
   <si>
+    <t>NO</t>
+  </si>
+  <si>
     <t>Done</t>
   </si>
   <si>
+    <t>Submit work early</t>
+  </si>
+  <si>
+    <t>Do separate tests for each story</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>using python3 instead of 2</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ready </t>
+  </si>
+  <si>
     <t>Story Description</t>
   </si>
   <si>
@@ -548,62 +575,65 @@
   </si>
   <si>
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="m/d"/>
+    <numFmt numFmtId="60" formatCode="0.0"/>
+    <numFmt numFmtId="61" formatCode="mmm d"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Cambria"/>
+      <name val="Helvetica"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="11"/>
-      <name val="Verdana"/>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Cambria"/>
     </font>
   </fonts>
   <fills count="3">
@@ -644,154 +674,106 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="61" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="13">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF888888"/>
-      <rgbColor rgb="FF4A7EBB"/>
-      <rgbColor rgb="00F20884"/>
-      <rgbColor rgb="0000ABEA"/>
-      <rgbColor rgb="00900000"/>
-      <rgbColor rgb="00006411"/>
-      <rgbColor rgb="00000090"/>
-      <rgbColor rgb="0090713A"/>
-      <rgbColor rgb="004600A5"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ff888888"/>
+      <rgbColor rgb="ff4a7ebb"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="18"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -800,10 +782,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.3645800000000006E-2"/>
-          <c:y val="6.0070699999999998E-2"/>
-          <c:w val="0.911354"/>
-          <c:h val="0.83019299999999996"/>
+          <c:x val="0.0841985"/>
+          <c:y val="0.0608311"/>
+          <c:w val="0.910802"/>
+          <c:h val="0.828202"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -816,6 +798,9 @@
             <c:v>Series1</c:v>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln w="28575" cap="flat">
               <a:solidFill>
                 <a:srgbClr val="4A7EBB"/>
@@ -827,7 +812,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -842,70 +827,91 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
+            <c:strRef>
+              <c:f>'Burndown'!$A$2:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40947</c:v>
+                  <c:v>2/9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40961</c:v>
+                  <c:v>2/23</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="d\-mmm">
-                  <c:v>40982</c:v>
+                <c:pt idx="2">
+                  <c:v>15-Mar</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="3">
+                  <c:v>Apr 5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>'Burndown'!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>13.000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-32A8-4804-BF13-24DEC399267B}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2107830952"/>
-        <c:axId val="2107827928"/>
+        <c:axId val="2094734552"/>
+        <c:axId val="2094734553"/>
       </c:lineChart>
-      <c:dateAx>
-        <c:axId val="2107830952"/>
+      <c:catAx>
+        <c:axId val="2094734552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -923,24 +929,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107827928"/>
+        <c:crossAx val="2094734553"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:lblAlgn val="ctr"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="2107827928"/>
+        <c:axId val="2094734553"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,17 +980,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107830952"/>
+        <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="6"/>
@@ -1004,7 +1008,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1019,41 +1022,36 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>510978</xdr:colOff>
+      <xdr:colOff>508853</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>109574</xdr:colOff>
+      <xdr:colOff>107643</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>97293</xdr:rowOff>
+      <xdr:rowOff>68222</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="1321653" y="1715049"/>
+        <a:ext cx="3815191" cy="2296524"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1063,7 +1061,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1189,7 +1187,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1198,7 +1196,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1207,7 +1205,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1281,7 +1279,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1289,7 +1287,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1308,7 +1306,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1338,7 +1336,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1364,7 +1362,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1388,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1416,7 +1414,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1442,7 +1440,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1468,7 +1466,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1494,7 +1492,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1520,7 +1518,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1546,7 +1544,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1559,15 +1557,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1582,7 +1574,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1590,7 +1582,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1609,7 +1601,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1635,7 +1627,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1661,7 +1653,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1687,7 +1679,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1713,7 +1705,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1739,7 +1731,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1765,7 +1757,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1791,7 +1783,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1817,7 +1809,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1843,7 +1835,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1856,15 +1848,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1878,7 +1864,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1897,7 +1883,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1927,7 +1913,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1953,7 +1939,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1979,7 +1965,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2005,7 +1991,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2031,7 +2017,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2057,7 +2043,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2083,7 +2069,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2109,7 +2095,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2135,7 +2121,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2148,147 +2134,140 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.3046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.35156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.15234375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3828125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3516" style="1" customWidth="1"/>
     <col min="6" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2297,7 +2276,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2305,379 +2284,401 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV25"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.3046875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.69140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.3828125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="6.69140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.69140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.35156" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.67188" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.3516" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.67188" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.67188" style="5" customWidth="1"/>
     <col min="6" max="256" width="11" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>34</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" t="s" s="4">
+        <v>5</v>
+      </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s" s="4">
         <v>36</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" t="s" s="4">
+        <v>10</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s" s="4">
         <v>37</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s" s="4">
         <v>38</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" t="s" s="4">
+        <v>10</v>
+      </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3">
         <v>3</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s" s="4">
         <v>46</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="3">
         <v>3</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s" s="4">
         <v>49</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s" s="4">
         <v>50</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="3">
         <v>2</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="3">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" t="s" s="4">
         <v>5</v>
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" s="3">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s" s="4">
         <v>55</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s" s="4">
         <v>56</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" t="s" s="4">
+        <v>15</v>
+      </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="3">
         <v>2</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="3">
         <v>2</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s" s="4">
         <v>64</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="3">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="3">
         <v>3</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s" s="4">
         <v>67</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s" s="4">
         <v>68</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s" s="4">
         <v>69</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s" s="4">
         <v>70</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" t="s" s="4">
+        <v>5</v>
+      </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="3">
         <v>3</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="s" s="4">
         <v>15</v>
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" s="3">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s" s="4">
         <v>73</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" t="s" s="4">
+        <v>15</v>
+      </c>
       <c r="E25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2685,46 +2686,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV26"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.69140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.3828125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.3828125" style="6" customWidth="1"/>
-    <col min="7" max="256" width="11" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.6719" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.3516" style="6" customWidth="1"/>
+    <col min="4" max="4" width="7.17188" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.85156" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.3516" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11" style="6" customWidth="1"/>
+    <col min="8" max="256" width="11" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" ht="13.5" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>80</v>
       </c>
+      <c r="F1" t="s" s="2">
+        <v>81</v>
+      </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="7">
         <v>40947</v>
       </c>
@@ -2739,7 +2739,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="7">
         <v>40961</v>
       </c>
@@ -2758,12 +2758,12 @@
       </c>
       <c r="F3" s="8">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>125</v>
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" s="9">
         <v>40982</v>
       </c>
       <c r="B4" s="3">
@@ -2780,20 +2780,33 @@
       </c>
       <c r="F4" s="8">
         <f>(D4-D3)/E4*60</f>
-        <v>76.599999999999994</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+    <row r="5" ht="13.5" customHeight="1">
+      <c r="A5" s="10">
+        <v>41003</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>753</v>
+      </c>
+      <c r="E5" s="3">
+        <v>116</v>
+      </c>
+      <c r="F5" s="8">
+        <f>(D5-D4)/E5*60</f>
+        <v>62.06896551724138</v>
+      </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2802,7 +2815,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2811,7 +2824,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2820,7 +2833,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2829,7 +2842,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2838,7 +2851,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2847,7 +2860,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2856,7 +2869,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2865,7 +2878,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2874,7 +2887,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2883,7 +2896,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2892,7 +2905,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2901,7 +2914,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2910,7 +2923,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2919,7 +2932,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2928,7 +2941,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2937,7 +2950,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2946,7 +2959,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2955,7 +2968,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2964,7 +2977,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2973,7 +2986,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2984,7 +2997,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2993,63 +3006,62 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV19"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.69140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="24.3828125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="6.69140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11" style="9" customWidth="1"/>
-    <col min="5" max="6" width="10.3046875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8.3828125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="9.3046875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="10.69140625" style="9" customWidth="1"/>
-    <col min="10" max="256" width="11" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.67188" style="11" customWidth="1"/>
+    <col min="2" max="2" width="24.3516" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.67188" style="11" customWidth="1"/>
+    <col min="4" max="4" width="11" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10.3516" style="11" customWidth="1"/>
+    <col min="6" max="6" width="10.3516" style="11" customWidth="1"/>
+    <col min="7" max="7" width="8.35156" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9.35156" style="11" customWidth="1"/>
+    <col min="9" max="9" width="10.6719" style="11" customWidth="1"/>
+    <col min="10" max="256" width="11" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s" s="12">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" t="s" s="13">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="F1" t="s" s="13">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" t="s" s="13">
         <v>84</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="H1" t="s" s="13">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="I1" t="s" s="13">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s" s="4">
         <v>10</v>
       </c>
       <c r="D2" s="3"/>
@@ -3065,18 +3077,18 @@
       <c r="H2" s="3">
         <v>30</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="I2" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s" s="4">
         <v>15</v>
       </c>
       <c r="D3" s="3"/>
@@ -3092,18 +3104,18 @@
       <c r="H3" s="3">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="I3" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s" s="4">
         <v>10</v>
       </c>
       <c r="D4" s="3"/>
@@ -3119,18 +3131,18 @@
       <c r="H4" s="3">
         <v>60</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="I4" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s" s="4">
         <v>15</v>
       </c>
       <c r="D5" s="3"/>
@@ -3146,18 +3158,18 @@
       <c r="H5" s="3">
         <v>40</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="I5" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D6" s="3"/>
@@ -3173,18 +3185,18 @@
       <c r="H6" s="3">
         <v>60</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="I6" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D7" s="3"/>
@@ -3200,13 +3212,13 @@
       <c r="H7" s="3">
         <v>5</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="12"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -3215,9 +3227,9 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="12"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -3226,9 +3238,9 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="12"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -3237,7 +3249,644 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" ht="15" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" ht="15" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" s="3"/>
+      <c r="B13" t="s" s="12">
+        <v>88</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" s="3"/>
+      <c r="B15" t="s" s="12">
+        <v>89</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" t="s" s="12">
+        <v>90</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="11" style="15" customWidth="1"/>
+    <col min="2" max="2" width="24.6719" style="15" customWidth="1"/>
+    <col min="3" max="3" width="11" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11" style="15" customWidth="1"/>
+    <col min="7" max="7" width="11" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11" style="15" customWidth="1"/>
+    <col min="9" max="9" width="11" style="15" customWidth="1"/>
+    <col min="10" max="256" width="11" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s" s="12">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s" s="13">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s" s="13">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s" s="13">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s" s="13">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s" s="13">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>91</v>
+      </c>
+      <c r="E2" s="3">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s" s="4">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s" s="4">
+        <v>92</v>
+      </c>
+      <c r="E3" s="3">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3">
+        <v>120</v>
+      </c>
+      <c r="I3" t="s" s="4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45</v>
+      </c>
+      <c r="G4" s="3">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3">
+        <v>60</v>
+      </c>
+      <c r="G5" s="3">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E6" s="3">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>60</v>
+      </c>
+      <c r="G6" s="3">
+        <v>7</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E7" s="3">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="11" style="16" customWidth="1"/>
+    <col min="2" max="2" width="26.3516" style="16" customWidth="1"/>
+    <col min="3" max="3" width="11" style="16" customWidth="1"/>
+    <col min="4" max="4" width="11" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11" style="16" customWidth="1"/>
+    <col min="6" max="6" width="11" style="16" customWidth="1"/>
+    <col min="7" max="7" width="11" style="16" customWidth="1"/>
+    <col min="8" max="8" width="11" style="16" customWidth="1"/>
+    <col min="9" max="9" width="11" style="16" customWidth="1"/>
+    <col min="10" max="256" width="11" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s" s="12">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s" s="13">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s" s="13">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s" s="13">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s" s="13">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s" s="13">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E2" s="3">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45</v>
+      </c>
+      <c r="G2" s="3">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s" s="4">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E4" s="3">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3">
+        <v>28</v>
+      </c>
+      <c r="H4" s="3">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="4">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E5" s="3">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3">
+        <v>32</v>
+      </c>
+      <c r="H5" s="3">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E6" s="3">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s" s="4">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E7" s="3">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3">
+        <v>20</v>
+      </c>
+      <c r="H7" s="3">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" t="s" s="12">
+        <v>88</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="12"/>
       <c r="C11" s="3"/>
@@ -3248,9 +3897,11 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="12"/>
+      <c r="B12" t="s" s="12">
+        <v>89</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -3259,10 +3910,10 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="10" t="s">
-        <v>87</v>
+      <c r="B13" t="s" s="17">
+        <v>95</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3272,22 +3923,22 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="10"/>
+      <c r="B14" t="s" s="17">
+        <v>96</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="3"/>
-      <c r="B15" s="10" t="s">
-        <v>88</v>
-      </c>
+      <c r="B15" s="14"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3296,9 +3947,11 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" s="12"/>
+      <c r="B16" t="s" s="12">
+        <v>90</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -3307,9 +3960,11 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="12"/>
+      <c r="B17" t="s" s="12">
+        <v>97</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -3318,7 +3973,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="12"/>
       <c r="C18" s="3"/>
@@ -3329,247 +3984,191 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="13" customWidth="1"/>
-    <col min="2" max="2" width="24.69140625" style="13" customWidth="1"/>
-    <col min="3" max="256" width="11" style="13" customWidth="1"/>
+    <col min="1" max="1" width="11" style="18" customWidth="1"/>
+    <col min="2" max="2" width="11" style="18" customWidth="1"/>
+    <col min="3" max="3" width="11" style="18" customWidth="1"/>
+    <col min="4" max="4" width="11" style="18" customWidth="1"/>
+    <col min="5" max="5" width="11" style="18" customWidth="1"/>
+    <col min="6" max="6" width="11" style="18" customWidth="1"/>
+    <col min="7" max="7" width="11" style="18" customWidth="1"/>
+    <col min="8" max="8" width="11" style="18" customWidth="1"/>
+    <col min="9" max="9" width="11" style="18" customWidth="1"/>
+    <col min="10" max="256" width="11" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s" s="12">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" t="s" s="13">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="F1" t="s" s="13">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" t="s" s="13">
         <v>84</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="H1" t="s" s="13">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>171</v>
+      <c r="I1" t="s" s="13">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>98</v>
       </c>
       <c r="E2" s="3">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3">
         <v>30</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" t="s" s="4">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="E3" s="3">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3">
         <v>20</v>
       </c>
-      <c r="H2" s="3">
-        <v>70</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s" s="4">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="E4" s="3">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3">
+        <v>60</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" t="s" s="4">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="3">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="D5" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="E5" s="3">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3">
         <v>30</v>
       </c>
-      <c r="G3" s="3">
-        <v>30</v>
-      </c>
-      <c r="H3" s="3">
-        <v>120</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5</v>
-      </c>
-      <c r="F4" s="3">
-        <v>45</v>
-      </c>
-      <c r="G4" s="3">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3">
-        <v>48</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="3">
-        <v>20</v>
-      </c>
-      <c r="F5" s="3">
-        <v>60</v>
-      </c>
-      <c r="G5" s="3">
-        <v>28</v>
-      </c>
-      <c r="H5" s="3">
-        <v>30</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>91</v>
+      <c r="D6" t="s" s="4">
+        <v>98</v>
       </c>
       <c r="E6" s="3">
         <v>20</v>
       </c>
       <c r="F6" s="3">
-        <v>60</v>
-      </c>
-      <c r="G6" s="3">
-        <v>7</v>
-      </c>
-      <c r="H6" s="3">
-        <v>45</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>91</v>
+      <c r="D7" t="s" s="4">
+        <v>98</v>
       </c>
       <c r="E7" s="3">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3">
-        <v>20</v>
-      </c>
-      <c r="G7" s="3">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>25</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3580,7 +4179,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3591,7 +4190,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3604,367 +4203,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11" style="14" customWidth="1"/>
-    <col min="2" max="2" width="26.3828125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="256" width="11" style="14" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="3">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3">
-        <v>45</v>
-      </c>
-      <c r="G2" s="3">
-        <v>8</v>
-      </c>
-      <c r="H2" s="3">
-        <v>45</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="3">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3">
-        <v>45</v>
-      </c>
-      <c r="G3" s="3">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3">
-        <v>30</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="256" width="11" style="15" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3972,581 +4211,583 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV43"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="16" customWidth="1"/>
-    <col min="2" max="2" width="24.3828125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="49.3046875" style="16" customWidth="1"/>
-    <col min="4" max="256" width="11" style="16" customWidth="1"/>
+    <col min="1" max="1" width="11" style="19" customWidth="1"/>
+    <col min="2" max="2" width="24.3516" style="19" customWidth="1"/>
+    <col min="3" max="3" width="49.3516" style="19" customWidth="1"/>
+    <col min="4" max="4" width="11" style="19" customWidth="1"/>
+    <col min="5" max="5" width="11" style="19" customWidth="1"/>
+    <col min="6" max="256" width="11" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>92</v>
+      <c r="C1" t="s" s="12">
+        <v>99</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>93</v>
+      <c r="C2" t="s" s="20">
+        <v>100</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>94</v>
+      <c r="C3" t="s" s="20">
+        <v>101</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>95</v>
+      <c r="C4" t="s" s="20">
+        <v>102</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>34</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>96</v>
+      <c r="C5" t="s" s="20">
+        <v>103</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>36</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>97</v>
+      <c r="C6" t="s" s="20">
+        <v>104</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>37</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>38</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>98</v>
+      <c r="C7" t="s" s="20">
+        <v>105</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" ht="45" customHeight="1">
+      <c r="A8" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>99</v>
+      <c r="C8" t="s" s="20">
+        <v>106</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>100</v>
+      <c r="C9" t="s" s="20">
+        <v>107</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>101</v>
+      <c r="C10" t="s" s="20">
+        <v>108</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s" s="4">
         <v>46</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>102</v>
+      <c r="C11" t="s" s="20">
+        <v>109</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>105</v>
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" t="s" s="4">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s" s="4">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s" s="20">
+        <v>112</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>108</v>
+    <row r="13" ht="45" customHeight="1">
+      <c r="A13" t="s" s="4">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s" s="4">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s" s="20">
+        <v>115</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>109</v>
+      <c r="C14" t="s" s="20">
+        <v>116</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" t="s" s="4">
         <v>49</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s" s="4">
         <v>50</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>110</v>
+      <c r="C15" t="s" s="20">
+        <v>117</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>113</v>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" t="s" s="4">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s" s="4">
+        <v>119</v>
+      </c>
+      <c r="C16" t="s" s="20">
+        <v>120</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>116</v>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" t="s" s="4">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s" s="4">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s" s="20">
+        <v>123</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>119</v>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="s" s="4">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s" s="20">
+        <v>126</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>120</v>
+      <c r="C19" t="s" s="20">
+        <v>127</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>121</v>
+      <c r="C20" t="s" s="20">
+        <v>128</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" t="s" s="4">
         <v>55</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s" s="4">
         <v>56</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>122</v>
+      <c r="C21" t="s" s="20">
+        <v>129</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="22" ht="30" customHeight="1">
+      <c r="A22" t="s" s="4">
         <v>57</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>123</v>
+      <c r="C22" t="s" s="20">
+        <v>130</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="23" ht="30" customHeight="1">
+      <c r="A23" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>124</v>
+      <c r="C23" t="s" s="20">
+        <v>131</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>127</v>
+    <row r="24" ht="30" customHeight="1">
+      <c r="A24" t="s" s="4">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s" s="4">
+        <v>133</v>
+      </c>
+      <c r="C24" t="s" s="20">
+        <v>134</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>130</v>
+    <row r="25" ht="45" customHeight="1">
+      <c r="A25" t="s" s="4">
+        <v>135</v>
+      </c>
+      <c r="B25" t="s" s="4">
+        <v>136</v>
+      </c>
+      <c r="C25" t="s" s="20">
+        <v>137</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="26" ht="30" customHeight="1">
+      <c r="A26" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>131</v>
+      <c r="C26" t="s" s="20">
+        <v>138</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>134</v>
+    <row r="27" ht="75" customHeight="1">
+      <c r="A27" t="s" s="4">
+        <v>139</v>
+      </c>
+      <c r="B27" t="s" s="4">
+        <v>140</v>
+      </c>
+      <c r="C27" t="s" s="20">
+        <v>141</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s" s="4">
         <v>64</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>135</v>
+      <c r="C28" t="s" s="20">
+        <v>142</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>136</v>
+      <c r="C29" t="s" s="20">
+        <v>143</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>139</v>
+    <row r="30" ht="15" customHeight="1">
+      <c r="A30" t="s" s="4">
+        <v>144</v>
+      </c>
+      <c r="B30" t="s" s="4">
+        <v>145</v>
+      </c>
+      <c r="C30" t="s" s="20">
+        <v>146</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" t="s" s="4">
         <v>67</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s" s="4">
         <v>68</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>140</v>
+      <c r="C31" t="s" s="20">
+        <v>147</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>143</v>
+    <row r="32" ht="30" customHeight="1">
+      <c r="A32" t="s" s="4">
+        <v>148</v>
+      </c>
+      <c r="B32" t="s" s="4">
+        <v>149</v>
+      </c>
+      <c r="C32" t="s" s="20">
+        <v>150</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>146</v>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" t="s" s="4">
+        <v>151</v>
+      </c>
+      <c r="B33" t="s" s="4">
+        <v>152</v>
+      </c>
+      <c r="C33" t="s" s="20">
+        <v>153</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>149</v>
+    <row r="34" ht="30" customHeight="1">
+      <c r="A34" t="s" s="4">
+        <v>154</v>
+      </c>
+      <c r="B34" t="s" s="4">
+        <v>155</v>
+      </c>
+      <c r="C34" t="s" s="20">
+        <v>156</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>152</v>
+    <row r="35" ht="30" customHeight="1">
+      <c r="A35" t="s" s="4">
+        <v>157</v>
+      </c>
+      <c r="B35" t="s" s="4">
+        <v>158</v>
+      </c>
+      <c r="C35" t="s" s="20">
+        <v>159</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+    <row r="36" ht="30" customHeight="1">
+      <c r="A36" t="s" s="4">
         <v>69</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s" s="4">
         <v>70</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>153</v>
+      <c r="C36" t="s" s="20">
+        <v>160</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>156</v>
+    <row r="37" ht="30" customHeight="1">
+      <c r="A37" t="s" s="4">
+        <v>161</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>162</v>
+      </c>
+      <c r="C37" t="s" s="20">
+        <v>163</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>159</v>
+    <row r="38" ht="30" customHeight="1">
+      <c r="A38" t="s" s="4">
+        <v>164</v>
+      </c>
+      <c r="B38" t="s" s="4">
+        <v>165</v>
+      </c>
+      <c r="C38" t="s" s="20">
+        <v>166</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+    <row r="39" ht="30" customHeight="1">
+      <c r="A39" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>160</v>
+      <c r="C39" t="s" s="20">
+        <v>167</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>163</v>
+    <row r="40" ht="30" customHeight="1">
+      <c r="A40" t="s" s="4">
+        <v>168</v>
+      </c>
+      <c r="B40" t="s" s="4">
+        <v>169</v>
+      </c>
+      <c r="C40" t="s" s="20">
+        <v>170</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>166</v>
+    <row r="41" ht="30" customHeight="1">
+      <c r="A41" t="s" s="4">
+        <v>171</v>
+      </c>
+      <c r="B41" t="s" s="4">
+        <v>172</v>
+      </c>
+      <c r="C41" t="s" s="20">
+        <v>173</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>169</v>
+    <row r="42" ht="30" customHeight="1">
+      <c r="A42" t="s" s="4">
+        <v>174</v>
+      </c>
+      <c r="B42" t="s" s="4">
+        <v>175</v>
+      </c>
+      <c r="C42" t="s" s="20">
+        <v>176</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+    <row r="43" ht="30" customHeight="1">
+      <c r="A43" t="s" s="4">
         <v>73</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>170</v>
+      <c r="C43" t="s" s="20">
+        <v>177</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated US05 and US06 details
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezhil\Documents\agile\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="6"/>
   </bookViews>
@@ -16,7 +21,7 @@
     <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
     <sheet name="Stories" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="177">
   <si>
     <t>Initials</t>
   </si>
@@ -586,7 +591,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -642,7 +647,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -665,13 +670,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -703,6 +719,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -779,11 +796,19 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -796,10 +821,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0841985"/>
-          <c:y val="0.0608311"/>
+          <c:x val="8.4198499999999996E-2"/>
+          <c:y val="6.0831099999999999E-2"/>
           <c:w val="0.910802"/>
-          <c:h val="0.828202"/>
+          <c:h val="0.82820199999999999"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -845,16 +870,16 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40947.0</c:v>
+                  <c:v>40947</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40961.0</c:v>
+                  <c:v>40961</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="d\-mmm">
-                  <c:v>40982.0</c:v>
+                  <c:v>40982</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="mmm\ d">
-                  <c:v>41003.0</c:v>
+                  <c:v>41003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -866,21 +891,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-73AB-4A1A-803C-A5C48AFD1C0A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -985,8 +1015,8 @@
         <c:crossAx val="2141624440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="6.0"/>
-        <c:minorUnit val="3.0"/>
+        <c:majorUnit val="6"/>
+        <c:minorUnit val="3"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1018,7 +1048,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2168,17 +2198,17 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.3046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3046875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.15234375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" style="1" customWidth="1"/>
     <col min="6" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2195,14 +2225,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -2219,7 +2249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2236,7 +2266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2253,14 +2283,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2271,21 +2301,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2314,17 +2344,17 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.3046875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.69140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.3046875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.69140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.69140625" style="5" customWidth="1"/>
     <col min="6" max="256" width="11" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -2341,7 +2371,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>2</v>
       </c>
@@ -2356,7 +2386,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2371,7 +2401,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -2386,7 +2416,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2401,7 +2431,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2416,7 +2446,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -2431,7 +2461,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -2446,7 +2476,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -2461,7 +2491,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -2476,7 +2506,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -2491,7 +2521,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -2506,7 +2536,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>3</v>
       </c>
@@ -2521,7 +2551,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2</v>
       </c>
@@ -2536,7 +2566,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -2551,7 +2581,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>4</v>
       </c>
@@ -2566,7 +2596,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -2581,7 +2611,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -2596,7 +2626,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -2611,7 +2641,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -2626,7 +2656,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -2641,7 +2671,7 @@
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>3</v>
       </c>
@@ -2656,7 +2686,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>4</v>
       </c>
@@ -2671,7 +2701,7 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>3</v>
       </c>
@@ -2686,7 +2716,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>4</v>
       </c>
@@ -2719,20 +2749,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.69140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.3046875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.3046875" style="6" customWidth="1"/>
     <col min="7" max="256" width="11" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.5" customHeight="1">
+    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>75</v>
       </c>
@@ -2753,7 +2783,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="13.5" customHeight="1">
+    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>40947</v>
       </c>
@@ -2768,7 +2798,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="13.5" customHeight="1">
+    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>40961</v>
       </c>
@@ -2791,7 +2821,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="13.5" customHeight="1">
+    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>40982</v>
       </c>
@@ -2813,7 +2843,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="13.5" customHeight="1">
+    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>41003</v>
       </c>
@@ -2835,7 +2865,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="13.5" customHeight="1">
+    <row r="6" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2844,7 +2874,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="13.5" customHeight="1">
+    <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2853,7 +2883,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="13.5" customHeight="1">
+    <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2862,7 +2892,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="13.5" customHeight="1">
+    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2871,7 +2901,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="13.5" customHeight="1">
+    <row r="10" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2880,7 +2910,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="13.5" customHeight="1">
+    <row r="11" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2889,7 +2919,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="13.5" customHeight="1">
+    <row r="12" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2898,7 +2928,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="13.5" customHeight="1">
+    <row r="13" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2907,7 +2937,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="13.5" customHeight="1">
+    <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2916,7 +2946,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="13.5" customHeight="1">
+    <row r="15" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2925,7 +2955,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="13.5" customHeight="1">
+    <row r="16" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2934,7 +2964,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="13.5" customHeight="1">
+    <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2943,7 +2973,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="13.5" customHeight="1">
+    <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2952,7 +2982,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="13.5" customHeight="1">
+    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2961,7 +2991,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1">
+    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2970,7 +3000,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="13.5" customHeight="1">
+    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2979,7 +3009,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="13.5" customHeight="1">
+    <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2988,7 +3018,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="13.5" customHeight="1">
+    <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2997,7 +3027,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="13.5" customHeight="1">
+    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3006,7 +3036,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="13.5" customHeight="1">
+    <row r="25" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -3015,7 +3045,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="13.5" customHeight="1">
+    <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3045,20 +3075,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="7.69140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="24.3046875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.69140625" style="11" customWidth="1"/>
     <col min="4" max="4" width="11" style="11" customWidth="1"/>
-    <col min="5" max="6" width="10.28515625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="11" customWidth="1"/>
+    <col min="5" max="6" width="10.3046875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="8.3046875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9.3046875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="10.69140625" style="11" customWidth="1"/>
     <col min="10" max="256" width="11" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -3087,7 +3117,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -3114,7 +3144,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>59</v>
       </c>
@@ -3141,7 +3171,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
@@ -3168,7 +3198,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
@@ -3195,7 +3225,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -3222,7 +3252,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -3249,7 +3279,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="14"/>
       <c r="C8" s="3"/>
@@ -3260,7 +3290,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="14"/>
       <c r="C9" s="3"/>
@@ -3271,7 +3301,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="14"/>
       <c r="C10" s="3"/>
@@ -3282,7 +3312,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="14"/>
       <c r="C11" s="3"/>
@@ -3293,7 +3323,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="14"/>
       <c r="C12" s="3"/>
@@ -3304,7 +3334,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="12" t="s">
         <v>87</v>
@@ -3317,7 +3347,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="12"/>
       <c r="C14" s="3"/>
@@ -3328,7 +3358,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="12" t="s">
         <v>88</v>
@@ -3341,7 +3371,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="14"/>
       <c r="C16" s="3"/>
@@ -3352,7 +3382,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="14"/>
       <c r="C17" s="3"/>
@@ -3363,7 +3393,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="14"/>
       <c r="C18" s="3"/>
@@ -3374,7 +3404,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1">
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="12" t="s">
         <v>89</v>
@@ -3407,14 +3437,14 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="15" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="24.69140625" style="15" customWidth="1"/>
     <col min="3" max="256" width="11" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -3443,7 +3473,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -3472,7 +3502,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
@@ -3501,7 +3531,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
@@ -3530,7 +3560,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>65</v>
       </c>
@@ -3559,7 +3589,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>63</v>
       </c>
@@ -3588,7 +3618,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -3617,7 +3647,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3628,7 +3658,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3639,7 +3669,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3668,16 +3698,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="16" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="26.3046875" style="16" customWidth="1"/>
     <col min="3" max="256" width="11" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -3706,7 +3738,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -3735,7 +3767,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -3764,7 +3796,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>45</v>
       </c>
@@ -3793,7 +3825,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>49</v>
       </c>
@@ -3822,7 +3854,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>67</v>
       </c>
@@ -3851,7 +3883,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>71</v>
       </c>
@@ -3880,7 +3912,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3891,7 +3923,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3902,7 +3934,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="12" t="s">
         <v>87</v>
@@ -3915,7 +3947,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="12"/>
       <c r="C11" s="3"/>
@@ -3926,7 +3958,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="12" t="s">
         <v>88</v>
@@ -3939,7 +3971,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="17" t="s">
         <v>94</v>
@@ -3952,7 +3984,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="17" t="s">
         <v>95</v>
@@ -3965,7 +3997,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="14"/>
       <c r="C15" s="3"/>
@@ -3976,7 +4008,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="12" t="s">
         <v>89</v>
@@ -3989,7 +4021,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="12" t="s">
         <v>96</v>
@@ -4002,7 +4034,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="12"/>
       <c r="C18" s="3"/>
@@ -4032,15 +4064,17 @@
   <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D5" sqref="D5:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="256" width="11" style="18" customWidth="1"/>
+    <col min="1" max="1" width="11" style="18" customWidth="1"/>
+    <col min="2" max="2" width="19.765625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="256" width="11" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -4069,10 +4103,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>15</v>
@@ -4090,16 +4126,18 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E3" s="3">
         <v>30</v>
@@ -4107,14 +4145,22 @@
       <c r="F3" s="3">
         <v>20</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
+      <c r="G3" s="3">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="B4" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>15</v>
@@ -4132,16 +4178,18 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E5" s="3">
         <v>35</v>
@@ -4159,55 +4207,65 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E6" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3">
         <v>30</v>
       </c>
       <c r="G6" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H6" s="3">
-        <v>18</v>
-      </c>
-      <c r="I6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E7" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3">
         <v>30</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="G7" s="3">
+        <v>40</v>
+      </c>
+      <c r="H7" s="3">
+        <v>30</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -4218,7 +4276,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4229,7 +4287,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4258,19 +4316,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="19" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="24.3046875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="49.3046875" style="19" customWidth="1"/>
     <col min="4" max="256" width="11" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -4283,7 +4341,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -4296,7 +4354,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -4309,7 +4367,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -4322,7 +4380,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1">
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -4335,7 +4393,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -4348,7 +4406,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>37</v>
       </c>
@@ -4361,7 +4419,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="45" customHeight="1">
+    <row r="8" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
@@ -4374,7 +4432,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1">
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -4387,7 +4445,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
@@ -4400,7 +4458,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1">
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>45</v>
       </c>
@@ -4413,7 +4471,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>109</v>
       </c>
@@ -4426,7 +4484,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="45" customHeight="1">
+    <row r="13" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>112</v>
       </c>
@@ -4439,7 +4497,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
@@ -4452,7 +4510,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
@@ -4465,7 +4523,7 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>117</v>
       </c>
@@ -4478,7 +4536,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>120</v>
       </c>
@@ -4491,7 +4549,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>123</v>
       </c>
@@ -4504,7 +4562,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>51</v>
       </c>
@@ -4517,7 +4575,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>53</v>
       </c>
@@ -4530,7 +4588,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>55</v>
       </c>
@@ -4543,7 +4601,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1">
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>57</v>
       </c>
@@ -4556,7 +4614,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1">
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
@@ -4569,7 +4627,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="30" customHeight="1">
+    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>131</v>
       </c>
@@ -4582,7 +4640,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="45" customHeight="1">
+    <row r="25" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>134</v>
       </c>
@@ -4595,7 +4653,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1">
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>61</v>
       </c>
@@ -4608,7 +4666,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="75" customHeight="1">
+    <row r="27" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>138</v>
       </c>
@@ -4621,7 +4679,7 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>63</v>
       </c>
@@ -4634,7 +4692,7 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
@@ -4647,7 +4705,7 @@
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>143</v>
       </c>
@@ -4660,7 +4718,7 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>67</v>
       </c>
@@ -4673,7 +4731,7 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1">
+    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>147</v>
       </c>
@@ -4686,7 +4744,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>150</v>
       </c>
@@ -4699,7 +4757,7 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1">
+    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>153</v>
       </c>
@@ -4712,7 +4770,7 @@
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="30" customHeight="1">
+    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>156</v>
       </c>
@@ -4725,7 +4783,7 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" ht="30" customHeight="1">
+    <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>69</v>
       </c>
@@ -4738,7 +4796,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1">
+    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>160</v>
       </c>
@@ -4751,7 +4809,7 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="30" customHeight="1">
+    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>163</v>
       </c>
@@ -4764,7 +4822,7 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" ht="30" customHeight="1">
+    <row r="39" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>71</v>
       </c>
@@ -4777,7 +4835,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" ht="30" customHeight="1">
+    <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>167</v>
       </c>
@@ -4790,7 +4848,7 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="30" customHeight="1">
+    <row r="41" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>170</v>
       </c>
@@ -4803,7 +4861,7 @@
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="30" customHeight="1">
+    <row r="42" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>173</v>
       </c>
@@ -4816,7 +4874,7 @@
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="30" customHeight="1">
+    <row r="43" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>73</v>
       </c>

</xml_diff>